<commit_message>
comparer calculates ROI per league
</commit_message>
<xml_diff>
--- a/UEFA.xlsx
+++ b/UEFA.xlsx
@@ -599,98 +599,98 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Israel</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>Belgium</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Italy</t>
-        </is>
-      </c>
       <c r="D2" t="n">
-        <v>35.19</v>
+        <v>28.92</v>
       </c>
       <c r="E2" t="n">
-        <v>21.72</v>
+        <v>26.18</v>
       </c>
       <c r="F2" t="n">
-        <v>43.09</v>
+        <v>44.9</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>56.91</v>
+        <v>55.1</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>78.28</v>
-      </c>
-      <c r="J2" t="n">
-        <v>64.81</v>
+        <v>73.81999999999999</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>71.08</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>76.45</v>
+        <v>73.8</v>
       </c>
       <c r="L2" t="n">
-        <v>54.63</v>
-      </c>
-      <c r="M2" t="n">
-        <v>67.7</v>
+        <v>48.63</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>73.19</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>83.70999999999999</v>
+        <v>87.47</v>
       </c>
       <c r="O2" t="n">
-        <v>56.25</v>
+        <v>52.67</v>
       </c>
       <c r="P2" t="n">
-        <v>4.43</v>
+        <v>26.11</v>
       </c>
       <c r="Q2" t="n">
-        <v>44.5</v>
+        <v>57.34</v>
       </c>
       <c r="R2" t="n">
-        <v>50.03</v>
+        <v>16.37</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
           <t>0-0</t>
         </is>
       </c>
-      <c r="T2" t="n">
-        <v>48.93</v>
+      <c r="T2" s="2" t="n">
+        <v>83.45</v>
       </c>
       <c r="U2" t="n">
-        <v>54.46</v>
+        <v>42.48</v>
       </c>
       <c r="V2" s="2" t="n">
-        <v>94.53</v>
-      </c>
-      <c r="W2" s="2" t="n">
-        <v>73.29000000000001</v>
+        <v>73.71000000000001</v>
+      </c>
+      <c r="W2" t="n">
+        <v>65.54000000000001</v>
       </c>
       <c r="X2" t="n">
-        <v>41.33</v>
-      </c>
-      <c r="Y2" s="2" t="n">
-        <v>73.95</v>
+        <v>49.58</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>67.93000000000001</v>
       </c>
       <c r="Z2" s="2" t="n">
-        <v>78.16</v>
+        <v>77.27</v>
       </c>
       <c r="AA2" t="n">
-        <v>38.91</v>
+        <v>31.47</v>
       </c>
       <c r="AB2" t="n">
-        <v>44.93</v>
+        <v>43.59</v>
       </c>
       <c r="AC2" s="2" t="n">
-        <v>84.65000000000001</v>
+        <v>89.27</v>
       </c>
       <c r="AD2" s="2" t="n">
-        <v>80.34</v>
+        <v>81.34999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -701,98 +701,98 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>France</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Israel</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>89.11</v>
+      <c r="D3" t="n">
+        <v>60.66</v>
       </c>
       <c r="E3" t="n">
-        <v>4.45</v>
+        <v>21.14</v>
       </c>
       <c r="F3" t="n">
-        <v>2.68</v>
+        <v>18.17</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>4-0</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="H3" s="2" t="n">
-        <v>93.56</v>
+        <v>81.8</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>91.79000000000001</v>
+        <v>78.83</v>
       </c>
       <c r="J3" t="n">
-        <v>7.130000000000001</v>
+        <v>39.31</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>92.70999999999999</v>
-      </c>
-      <c r="L3" s="2" t="n">
-        <v>85.73</v>
+        <v>81.20999999999999</v>
+      </c>
+      <c r="L3" t="n">
+        <v>59.18</v>
       </c>
       <c r="M3" t="n">
-        <v>23.14</v>
-      </c>
-      <c r="N3" t="n">
-        <v>39.75</v>
+        <v>63.17</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>80.34999999999999</v>
       </c>
       <c r="O3" t="n">
-        <v>52.47</v>
+        <v>55.98</v>
       </c>
       <c r="P3" t="n">
-        <v>63.09</v>
+        <v>47.25</v>
       </c>
       <c r="Q3" t="n">
-        <v>31.78</v>
+        <v>47.47</v>
       </c>
       <c r="R3" t="n">
-        <v>1.07</v>
+        <v>4.61</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>2-0</t>
+          <t>0-0</t>
         </is>
       </c>
       <c r="T3" s="2" t="n">
-        <v>94.87</v>
+        <v>94.72</v>
       </c>
       <c r="U3" t="n">
+        <v>51.86</v>
+      </c>
+      <c r="V3" t="n">
+        <v>52.08</v>
+      </c>
+      <c r="W3" s="2" t="n">
+        <v>70.17</v>
+      </c>
+      <c r="X3" t="n">
+        <v>46.83</v>
+      </c>
+      <c r="Y3" s="2" t="n">
+        <v>87</v>
+      </c>
+      <c r="Z3" t="n">
         <v>64.16</v>
       </c>
-      <c r="V3" t="n">
-        <v>32.85</v>
-      </c>
-      <c r="W3" s="2" t="n">
-        <v>79.41</v>
-      </c>
-      <c r="X3" t="n">
-        <v>28.25</v>
-      </c>
-      <c r="Y3" s="2" t="n">
-        <v>95.06</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>53.37</v>
-      </c>
-      <c r="AA3" s="2" t="n">
-        <v>89.83</v>
+      <c r="AA3" t="n">
+        <v>60.51</v>
       </c>
       <c r="AB3" t="n">
-        <v>18.71</v>
+        <v>27.39</v>
       </c>
       <c r="AC3" t="n">
-        <v>18.01</v>
+        <v>66.52</v>
       </c>
       <c r="AD3" s="2" t="n">
-        <v>91.55</v>
+        <v>91.45</v>
       </c>
     </row>
     <row r="4">
@@ -803,98 +803,98 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>England</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>75.19</v>
+        <v>87.92</v>
       </c>
       <c r="E4" t="n">
-        <v>17.54</v>
+        <v>9.640000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>7.25</v>
+        <v>2.24</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="H4" s="2" t="n">
-        <v>92.72999999999999</v>
+        <v>97.56</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>82.44</v>
+        <v>90.16</v>
       </c>
       <c r="J4" t="n">
-        <v>24.79</v>
-      </c>
-      <c r="K4" t="n">
-        <v>63.81</v>
+        <v>11.88</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>80.16</v>
       </c>
       <c r="L4" t="n">
-        <v>37.99</v>
-      </c>
-      <c r="M4" s="2" t="n">
-        <v>81.73</v>
+        <v>57.82</v>
+      </c>
+      <c r="M4" t="n">
+        <v>64.38</v>
       </c>
       <c r="N4" s="2" t="n">
-        <v>92.64</v>
+        <v>81.27</v>
       </c>
       <c r="O4" t="n">
-        <v>24.25</v>
+        <v>23.18</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="2" t="n">
-        <v>100</v>
+        <v>67.67</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>31.68</v>
       </c>
       <c r="R4" t="n">
         <v>0</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>0-0</t>
+          <t>1-0</t>
         </is>
       </c>
       <c r="T4" s="2" t="n">
-        <v>100</v>
+        <v>99.34999999999999</v>
       </c>
       <c r="U4" t="n">
-        <v>0</v>
-      </c>
-      <c r="V4" s="2" t="n">
-        <v>100</v>
+        <v>67.67</v>
+      </c>
+      <c r="V4" t="n">
+        <v>31.68</v>
       </c>
       <c r="W4" t="n">
-        <v>0</v>
-      </c>
-      <c r="X4" s="2" t="n">
-        <v>100</v>
+        <v>67.67</v>
+      </c>
+      <c r="X4" t="n">
+        <v>68.09999999999999</v>
       </c>
       <c r="Y4" s="2" t="n">
-        <v>84.34</v>
+        <v>93.27</v>
       </c>
       <c r="Z4" t="n">
-        <v>29.89</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>55.32</v>
+        <v>24.74</v>
+      </c>
+      <c r="AA4" s="2" t="n">
+        <v>75.47</v>
       </c>
       <c r="AB4" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="AC4" s="2" t="n">
-        <v>71.58</v>
+        <v>3.36</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>48.62</v>
       </c>
       <c r="AD4" s="2" t="n">
-        <v>99.41</v>
+        <v>99.48</v>
       </c>
     </row>
     <row r="5">
@@ -905,60 +905,60 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>Finland</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>57.51</v>
+        <v>5.58</v>
       </c>
       <c r="E5" t="n">
-        <v>25.18</v>
-      </c>
-      <c r="F5" t="n">
-        <v>17.32</v>
+        <v>16.26</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>78.12</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>1-0</t>
-        </is>
-      </c>
-      <c r="H5" s="2" t="n">
-        <v>82.69</v>
+          <t>0-2</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>21.84</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>74.83</v>
-      </c>
-      <c r="J5" t="n">
-        <v>42.5</v>
-      </c>
-      <c r="K5" t="n">
-        <v>56.06</v>
+        <v>83.7</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>94.38000000000001</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>72.69</v>
       </c>
       <c r="L5" t="n">
-        <v>30.53</v>
+        <v>47.31</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>86.89</v>
+        <v>74.3</v>
       </c>
       <c r="N5" s="2" t="n">
-        <v>95.31</v>
+        <v>88.19</v>
       </c>
       <c r="O5" t="n">
-        <v>31.03</v>
+        <v>29.7</v>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>3.62</v>
       </c>
       <c r="Q5" t="n">
-        <v>45.36</v>
+        <v>56.5</v>
       </c>
       <c r="R5" t="n">
-        <v>54.51</v>
+        <v>39.83</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
@@ -966,37 +966,37 @@
         </is>
       </c>
       <c r="T5" t="n">
-        <v>45.36</v>
+        <v>60.12</v>
       </c>
       <c r="U5" t="n">
-        <v>54.51</v>
+        <v>43.45</v>
       </c>
       <c r="V5" s="2" t="n">
-        <v>99.87</v>
+        <v>96.33</v>
       </c>
       <c r="W5" t="n">
-        <v>54.51</v>
+        <v>50.55</v>
       </c>
       <c r="X5" s="2" t="n">
-        <v>81.22</v>
-      </c>
-      <c r="Y5" s="2" t="n">
-        <v>74.25</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>43.83</v>
+        <v>78.78</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>33.46</v>
+      </c>
+      <c r="Z5" s="2" t="n">
+        <v>88.43000000000001</v>
       </c>
       <c r="AA5" t="n">
-        <v>39.31</v>
+        <v>6.35</v>
       </c>
       <c r="AB5" t="n">
-        <v>11.43</v>
+        <v>63.53</v>
       </c>
       <c r="AC5" s="2" t="n">
-        <v>84.38</v>
-      </c>
-      <c r="AD5" s="2" t="n">
-        <v>97.91</v>
+        <v>99.13</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>63.34</v>
       </c>
     </row>
     <row r="6">
@@ -1007,98 +1007,98 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>Austria</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Austria</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
+          <t>Slovenia</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>88.27</v>
       </c>
       <c r="E6" t="n">
-        <v>8.140000000000001</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>91.75</v>
+        <v>6.72</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.2</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0-2</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>8.140000000000001</v>
+          <t>3-0</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>94.98999999999999</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>91.75</v>
-      </c>
-      <c r="J6" s="2" t="n">
-        <v>99.89</v>
+        <v>91.47</v>
+      </c>
+      <c r="J6" t="n">
+        <v>9.92</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>71.33</v>
-      </c>
-      <c r="L6" t="n">
-        <v>45.72</v>
-      </c>
-      <c r="M6" s="2" t="n">
-        <v>75.56999999999999</v>
-      </c>
-      <c r="N6" s="2" t="n">
-        <v>89</v>
+        <v>92.75</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>82.28</v>
+      </c>
+      <c r="M6" t="n">
+        <v>32.01</v>
+      </c>
+      <c r="N6" t="n">
+        <v>50.67</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>50.63</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>53.57</v>
       </c>
       <c r="Q6" t="n">
-        <v>34.85</v>
+        <v>34.01</v>
       </c>
       <c r="R6" t="n">
-        <v>64.7</v>
+        <v>5.76</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>0-1</t>
-        </is>
-      </c>
-      <c r="T6" t="n">
-        <v>34.85</v>
+          <t>1-1</t>
+        </is>
+      </c>
+      <c r="T6" s="2" t="n">
+        <v>87.58</v>
       </c>
       <c r="U6" t="n">
-        <v>64.7</v>
-      </c>
-      <c r="V6" s="2" t="n">
-        <v>99.55000000000001</v>
-      </c>
-      <c r="W6" t="n">
-        <v>64.7</v>
-      </c>
-      <c r="X6" s="2" t="n">
-        <v>71.58</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="2" t="n">
-        <v>91.75</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="2" t="n">
-        <v>71.33</v>
-      </c>
-      <c r="AC6" s="2" t="n">
-        <v>99.88</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>54.16</v>
+        <v>59.33</v>
+      </c>
+      <c r="V6" t="n">
+        <v>39.77</v>
+      </c>
+      <c r="W6" s="2" t="n">
+        <v>80.73</v>
+      </c>
+      <c r="X6" t="n">
+        <v>13.25</v>
+      </c>
+      <c r="Y6" s="2" t="n">
+        <v>96.13</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>51.67</v>
+      </c>
+      <c r="AA6" s="2" t="n">
+        <v>88.16</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>16.92</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="AD6" s="2" t="n">
+        <v>94.23999999999999</v>
       </c>
     </row>
     <row r="7">
@@ -1109,60 +1109,60 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Slovenia</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Norway</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>41.68</v>
+          <t>Kazakhstan</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>92.08</v>
       </c>
       <c r="E7" t="n">
-        <v>22.98</v>
+        <v>7.79</v>
       </c>
       <c r="F7" t="n">
-        <v>35.34</v>
+        <v>0</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>1-0</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>64.66</v>
+          <t>2-0</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>99.87</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>77.02000000000001</v>
+        <v>92.08</v>
       </c>
       <c r="J7" t="n">
-        <v>58.32000000000001</v>
+        <v>7.79</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>71.56</v>
+        <v>72.2</v>
       </c>
       <c r="L7" t="n">
-        <v>48.12</v>
+        <v>46.83</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>73.63</v>
+        <v>74.63</v>
       </c>
       <c r="N7" s="2" t="n">
-        <v>87.76000000000001</v>
+        <v>88.40000000000001</v>
       </c>
       <c r="O7" t="n">
-        <v>51.1</v>
+        <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>13.71</v>
+        <v>59.76</v>
       </c>
       <c r="Q7" t="n">
-        <v>60.64</v>
+        <v>39.98</v>
       </c>
       <c r="R7" t="n">
-        <v>25.62</v>
+        <v>0</v>
       </c>
       <c r="S7" t="inlineStr">
         <is>
@@ -1170,37 +1170,37 @@
         </is>
       </c>
       <c r="T7" s="2" t="n">
-        <v>74.34999999999999</v>
+        <v>99.73999999999999</v>
       </c>
       <c r="U7" t="n">
-        <v>39.33</v>
-      </c>
-      <c r="V7" s="2" t="n">
-        <v>86.26000000000001</v>
+        <v>59.76</v>
+      </c>
+      <c r="V7" t="n">
+        <v>39.98</v>
       </c>
       <c r="W7" t="n">
-        <v>54.82</v>
-      </c>
-      <c r="X7" t="n">
-        <v>68.77</v>
+        <v>59.76</v>
+      </c>
+      <c r="X7" s="2" t="n">
+        <v>76.64</v>
       </c>
       <c r="Y7" s="2" t="n">
-        <v>74.51000000000001</v>
-      </c>
-      <c r="Z7" s="2" t="n">
-        <v>70.81999999999999</v>
-      </c>
-      <c r="AA7" t="n">
-        <v>39.67</v>
+        <v>92.08</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="2" t="n">
+        <v>72.2</v>
       </c>
       <c r="AB7" t="n">
-        <v>34.88</v>
-      </c>
-      <c r="AC7" s="2" t="n">
-        <v>84.14</v>
+        <v>0</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>53.04</v>
       </c>
       <c r="AD7" s="2" t="n">
-        <v>87.25</v>
+        <v>99.87</v>
       </c>
     </row>
     <row r="8">
@@ -1211,98 +1211,98 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>Latvia</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>Armenia</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Faroe Islands</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>73.41</v>
+      <c r="D8" t="n">
+        <v>33.91</v>
       </c>
       <c r="E8" t="n">
-        <v>13.94</v>
+        <v>21.63</v>
       </c>
       <c r="F8" t="n">
-        <v>12.51</v>
+        <v>44.43</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2-0</t>
-        </is>
-      </c>
-      <c r="H8" s="2" t="n">
-        <v>87.34999999999999</v>
+          <t>1-1</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>55.53999999999999</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>85.92</v>
+        <v>78.34</v>
       </c>
       <c r="J8" t="n">
-        <v>26.45</v>
+        <v>66.06</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>85.67</v>
-      </c>
-      <c r="L8" t="n">
-        <v>68.39</v>
+        <v>88.62</v>
+      </c>
+      <c r="L8" s="2" t="n">
+        <v>71.7</v>
       </c>
       <c r="M8" t="n">
-        <v>52.93</v>
-      </c>
-      <c r="N8" s="2" t="n">
-        <v>71.90000000000001</v>
-      </c>
-      <c r="O8" t="n">
-        <v>55.57</v>
+        <v>49.08</v>
+      </c>
+      <c r="N8" t="n">
+        <v>68.41</v>
+      </c>
+      <c r="O8" s="2" t="n">
+        <v>71.06</v>
       </c>
       <c r="P8" t="n">
-        <v>15.84</v>
+        <v>8.32</v>
       </c>
       <c r="Q8" t="n">
-        <v>56.06</v>
+        <v>46.97</v>
       </c>
       <c r="R8" t="n">
-        <v>27.9</v>
+        <v>43.29</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
           <t>0-0</t>
         </is>
       </c>
-      <c r="T8" s="2" t="n">
-        <v>71.90000000000001</v>
+      <c r="T8" t="n">
+        <v>55.29</v>
       </c>
       <c r="U8" t="n">
-        <v>43.73999999999999</v>
+        <v>51.61</v>
       </c>
       <c r="V8" s="2" t="n">
-        <v>83.96000000000001</v>
-      </c>
-      <c r="W8" t="n">
-        <v>66.69</v>
+        <v>90.25999999999999</v>
+      </c>
+      <c r="W8" s="2" t="n">
+        <v>76.08</v>
       </c>
       <c r="X8" t="n">
-        <v>48.6</v>
+        <v>29.79</v>
       </c>
       <c r="Y8" s="2" t="n">
-        <v>92.33</v>
-      </c>
-      <c r="Z8" t="n">
-        <v>61.14</v>
-      </c>
-      <c r="AA8" s="2" t="n">
-        <v>72.86</v>
+        <v>82.17</v>
+      </c>
+      <c r="Z8" s="2" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>51.45</v>
       </c>
       <c r="AB8" t="n">
-        <v>24.45</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>52.18</v>
-      </c>
-      <c r="AD8" s="2" t="n">
-        <v>92.78</v>
+        <v>59.11</v>
+      </c>
+      <c r="AC8" s="2" t="n">
+        <v>75.02</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>67.93000000000001</v>
       </c>
     </row>
     <row r="9">
@@ -1318,55 +1318,55 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Latvia</t>
-        </is>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>92.87</v>
+          <t>Faroe Islands</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>67.23</v>
       </c>
       <c r="E9" t="n">
-        <v>5.91</v>
+        <v>29.66</v>
       </c>
       <c r="F9" t="n">
-        <v>0.87</v>
+        <v>3.11</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2-0</t>
+          <t>1-0</t>
         </is>
       </c>
       <c r="H9" s="2" t="n">
-        <v>98.78</v>
+        <v>96.89</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>93.74000000000001</v>
+        <v>70.34</v>
       </c>
       <c r="J9" t="n">
-        <v>6.78</v>
-      </c>
-      <c r="K9" s="2" t="n">
-        <v>80.59</v>
+        <v>32.77</v>
+      </c>
+      <c r="K9" t="n">
+        <v>39.07</v>
       </c>
       <c r="L9" t="n">
-        <v>58.95</v>
-      </c>
-      <c r="M9" t="n">
-        <v>63.09</v>
+        <v>15.42</v>
+      </c>
+      <c r="M9" s="2" t="n">
+        <v>95.19</v>
       </c>
       <c r="N9" s="2" t="n">
-        <v>80.28</v>
+        <v>98.77</v>
       </c>
       <c r="O9" t="n">
-        <v>9.98</v>
+        <v>7.33</v>
       </c>
       <c r="P9" t="n">
-        <v>27.94</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>67.61</v>
+        <v>3.25</v>
+      </c>
+      <c r="Q9" s="2" t="n">
+        <v>82.86</v>
       </c>
       <c r="R9" t="n">
-        <v>4.44</v>
+        <v>13.89</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
@@ -1374,37 +1374,37 @@
         </is>
       </c>
       <c r="T9" s="2" t="n">
-        <v>95.55</v>
+        <v>86.11</v>
       </c>
       <c r="U9" t="n">
-        <v>32.38</v>
+        <v>17.14</v>
       </c>
       <c r="V9" s="2" t="n">
-        <v>72.05</v>
+        <v>96.75</v>
       </c>
       <c r="W9" t="n">
-        <v>36.38</v>
+        <v>18.2</v>
       </c>
       <c r="X9" s="2" t="n">
-        <v>89.84</v>
+        <v>97.66</v>
       </c>
       <c r="Y9" s="2" t="n">
-        <v>94.45999999999999</v>
+        <v>71.06999999999999</v>
       </c>
       <c r="Z9" t="n">
-        <v>10.75</v>
-      </c>
-      <c r="AA9" s="2" t="n">
-        <v>79.11</v>
+        <v>10.24</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>35.19</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="AC9" t="n">
-        <v>43.25</v>
+        <v>0.54</v>
+      </c>
+      <c r="AC9" s="2" t="n">
+        <v>87.06</v>
       </c>
       <c r="AD9" s="2" t="n">
-        <v>99.63</v>
+        <v>99.98</v>
       </c>
     </row>
     <row r="10">
@@ -1415,60 +1415,60 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>Croatia</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>Portugal</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Poland</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>81.56999999999999</v>
+      <c r="D10" t="n">
+        <v>21.43</v>
       </c>
       <c r="E10" t="n">
-        <v>10.09</v>
+        <v>31.33</v>
       </c>
       <c r="F10" t="n">
-        <v>7.81</v>
+        <v>47.24</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>3-0</t>
-        </is>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>91.66</v>
-      </c>
-      <c r="I10" s="2" t="n">
-        <v>89.38</v>
-      </c>
-      <c r="J10" t="n">
-        <v>17.9</v>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>90.02</v>
-      </c>
-      <c r="L10" s="2" t="n">
-        <v>76.39</v>
-      </c>
-      <c r="M10" t="n">
-        <v>42.37</v>
-      </c>
-      <c r="N10" t="n">
-        <v>61.9</v>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>52.76</v>
+      </c>
+      <c r="I10" t="n">
+        <v>68.67</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>78.56999999999999</v>
+      </c>
+      <c r="K10" t="n">
+        <v>55.45</v>
+      </c>
+      <c r="L10" t="n">
+        <v>28.35</v>
+      </c>
+      <c r="M10" s="2" t="n">
+        <v>88.27</v>
+      </c>
+      <c r="N10" s="2" t="n">
+        <v>95.97</v>
       </c>
       <c r="O10" t="n">
-        <v>55.54</v>
+        <v>34.34</v>
       </c>
       <c r="P10" t="n">
-        <v>43.03</v>
+        <v>20.63</v>
       </c>
       <c r="Q10" t="n">
-        <v>48.17</v>
+        <v>52.86</v>
       </c>
       <c r="R10" t="n">
-        <v>7.92</v>
+        <v>25.8</v>
       </c>
       <c r="S10" t="inlineStr">
         <is>
@@ -1476,37 +1476,37 @@
         </is>
       </c>
       <c r="T10" s="2" t="n">
-        <v>91.2</v>
+        <v>73.48999999999999</v>
       </c>
       <c r="U10" t="n">
-        <v>50.95</v>
-      </c>
-      <c r="V10" t="n">
-        <v>56.09</v>
+        <v>46.43</v>
+      </c>
+      <c r="V10" s="2" t="n">
+        <v>78.66</v>
       </c>
       <c r="W10" s="2" t="n">
-        <v>73.5</v>
+        <v>74.45999999999999</v>
       </c>
       <c r="X10" t="n">
-        <v>37.64</v>
-      </c>
-      <c r="Y10" s="2" t="n">
-        <v>95.22</v>
+        <v>30.53</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>49.57</v>
       </c>
       <c r="Z10" t="n">
-        <v>58.7</v>
-      </c>
-      <c r="AA10" s="2" t="n">
-        <v>81.8</v>
+        <v>68.91</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>15.05</v>
       </c>
       <c r="AB10" t="n">
-        <v>22.33</v>
-      </c>
-      <c r="AC10" t="n">
-        <v>38.86</v>
+        <v>32.58</v>
+      </c>
+      <c r="AC10" s="2" t="n">
+        <v>96.77</v>
       </c>
       <c r="AD10" s="2" t="n">
-        <v>93.34999999999999</v>
+        <v>88.63</v>
       </c>
     </row>
     <row r="11">
@@ -1517,60 +1517,60 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>Poland</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>Scotland</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Croatia</t>
-        </is>
-      </c>
       <c r="D11" t="n">
-        <v>35.01</v>
+        <v>55.54</v>
       </c>
       <c r="E11" t="n">
-        <v>25.35</v>
+        <v>19.04</v>
       </c>
       <c r="F11" t="n">
-        <v>39.64</v>
+        <v>25.3</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>0-1</t>
-        </is>
-      </c>
-      <c r="H11" t="n">
-        <v>60.36</v>
+          <t>2-1</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>74.58</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>74.65000000000001</v>
+        <v>80.84</v>
       </c>
       <c r="J11" t="n">
-        <v>64.99000000000001</v>
-      </c>
-      <c r="K11" t="n">
-        <v>63.29</v>
-      </c>
-      <c r="L11" t="n">
-        <v>38.32</v>
-      </c>
-      <c r="M11" s="2" t="n">
-        <v>81.5</v>
-      </c>
-      <c r="N11" s="2" t="n">
-        <v>92.51000000000001</v>
-      </c>
-      <c r="O11" t="n">
-        <v>43.14</v>
+        <v>44.34</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>92</v>
+      </c>
+      <c r="L11" s="2" t="n">
+        <v>78.48</v>
+      </c>
+      <c r="M11" t="n">
+        <v>40.07</v>
+      </c>
+      <c r="N11" t="n">
+        <v>59.54</v>
+      </c>
+      <c r="O11" s="2" t="n">
+        <v>74.59</v>
       </c>
       <c r="P11" t="n">
-        <v>27.65</v>
+        <v>25.33</v>
       </c>
       <c r="Q11" t="n">
-        <v>54.29</v>
+        <v>60.17</v>
       </c>
       <c r="R11" t="n">
-        <v>17.69</v>
+        <v>14.45</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
@@ -1578,37 +1578,37 @@
         </is>
       </c>
       <c r="T11" s="2" t="n">
-        <v>81.94</v>
+        <v>85.5</v>
       </c>
       <c r="U11" t="n">
-        <v>45.34</v>
+        <v>39.78</v>
       </c>
       <c r="V11" s="2" t="n">
-        <v>71.98</v>
-      </c>
-      <c r="W11" s="2" t="n">
-        <v>70.84999999999999</v>
+        <v>74.62</v>
+      </c>
+      <c r="W11" t="n">
+        <v>57.56</v>
       </c>
       <c r="X11" t="n">
-        <v>39.95</v>
-      </c>
-      <c r="Y11" t="n">
-        <v>65.52</v>
-      </c>
-      <c r="Z11" t="n">
-        <v>68.56</v>
-      </c>
-      <c r="AA11" t="n">
-        <v>28.81</v>
+        <v>63.83</v>
+      </c>
+      <c r="Y11" s="2" t="n">
+        <v>91.63</v>
+      </c>
+      <c r="Z11" s="2" t="n">
+        <v>81.19</v>
+      </c>
+      <c r="AA11" s="2" t="n">
+        <v>71.06</v>
       </c>
       <c r="AB11" t="n">
-        <v>32.18</v>
-      </c>
-      <c r="AC11" s="2" t="n">
-        <v>90.73999999999999</v>
+        <v>49.87</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>54.5</v>
       </c>
       <c r="AD11" s="2" t="n">
-        <v>88.86</v>
+        <v>76.26000000000001</v>
       </c>
     </row>
     <row r="12">
@@ -1619,22 +1619,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>Serbia</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>Denmark</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Spain</t>
-        </is>
-      </c>
       <c r="D12" t="n">
-        <v>15.51</v>
+        <v>19.64</v>
       </c>
       <c r="E12" t="n">
-        <v>38.63</v>
+        <v>42.13</v>
       </c>
       <c r="F12" t="n">
-        <v>45.86</v>
+        <v>38.23</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1642,37 +1642,37 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>54.14</v>
+        <v>61.77</v>
       </c>
       <c r="I12" t="n">
-        <v>61.37</v>
+        <v>57.87</v>
       </c>
       <c r="J12" s="2" t="n">
-        <v>84.49000000000001</v>
+        <v>80.36</v>
       </c>
       <c r="K12" t="n">
-        <v>30.76</v>
+        <v>32.78</v>
       </c>
       <c r="L12" t="n">
-        <v>10.98</v>
+        <v>11.4</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>97.04000000000001</v>
+        <v>96.88</v>
       </c>
       <c r="N12" s="2" t="n">
-        <v>99.34999999999999</v>
+        <v>99.3</v>
       </c>
       <c r="O12" t="n">
-        <v>14.73</v>
+        <v>18.56</v>
       </c>
       <c r="P12" t="n">
-        <v>9.09</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>63.1</v>
+        <v>10.63</v>
+      </c>
+      <c r="Q12" s="2" t="n">
+        <v>79.68000000000001</v>
       </c>
       <c r="R12" t="n">
-        <v>27.79</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
@@ -1680,37 +1680,37 @@
         </is>
       </c>
       <c r="T12" s="2" t="n">
-        <v>72.19</v>
+        <v>90.31</v>
       </c>
       <c r="U12" t="n">
-        <v>36.88</v>
+        <v>20.33</v>
       </c>
       <c r="V12" s="2" t="n">
-        <v>90.89</v>
+        <v>89.38000000000001</v>
       </c>
       <c r="W12" t="n">
-        <v>46.64</v>
+        <v>22.93</v>
       </c>
       <c r="X12" s="2" t="n">
-        <v>79.84999999999999</v>
+        <v>95.67</v>
       </c>
       <c r="Y12" t="n">
-        <v>28.54</v>
+        <v>35.53</v>
       </c>
       <c r="Z12" t="n">
-        <v>55.68</v>
+        <v>51.83</v>
       </c>
       <c r="AA12" t="n">
-        <v>4.53</v>
+        <v>7.23</v>
       </c>
       <c r="AB12" t="n">
-        <v>19.62</v>
+        <v>16.65</v>
       </c>
       <c r="AC12" s="2" t="n">
-        <v>99.51000000000001</v>
+        <v>98.98</v>
       </c>
       <c r="AD12" s="2" t="n">
-        <v>95.06</v>
+        <v>96.2</v>
       </c>
     </row>
     <row r="13">
@@ -1721,98 +1721,98 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>Spain</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>Switzerland</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Serbia</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>48.63</v>
+      <c r="D13" s="2" t="n">
+        <v>89</v>
       </c>
       <c r="E13" t="n">
-        <v>23.51</v>
+        <v>1.54</v>
       </c>
       <c r="F13" t="n">
-        <v>27.85</v>
+        <v>0.39</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>5-0</t>
         </is>
       </c>
       <c r="H13" s="2" t="n">
-        <v>72.14</v>
+        <v>90.54000000000001</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>76.48</v>
+        <v>89.39</v>
       </c>
       <c r="J13" t="n">
-        <v>51.36</v>
-      </c>
-      <c r="K13" t="n">
-        <v>67.36</v>
-      </c>
-      <c r="L13" t="n">
-        <v>42.91</v>
-      </c>
-      <c r="M13" s="2" t="n">
-        <v>77.97</v>
-      </c>
-      <c r="N13" s="2" t="n">
-        <v>90.47</v>
+        <v>1.93</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>88.75</v>
+      </c>
+      <c r="L13" s="2" t="n">
+        <v>83.38</v>
+      </c>
+      <c r="M13" t="n">
+        <v>17.77</v>
+      </c>
+      <c r="N13" t="n">
+        <v>32.38</v>
       </c>
       <c r="O13" t="n">
-        <v>45.63</v>
+        <v>30.27</v>
       </c>
       <c r="P13" t="n">
-        <v>26.18</v>
+        <v>68.51000000000001</v>
       </c>
       <c r="Q13" t="n">
-        <v>59.58</v>
+        <v>22.1</v>
       </c>
       <c r="R13" t="n">
-        <v>14.18</v>
+        <v>-0.33</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>0-0</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="T13" s="2" t="n">
-        <v>85.75999999999999</v>
+        <v>90.61000000000001</v>
       </c>
       <c r="U13" t="n">
-        <v>40.36</v>
-      </c>
-      <c r="V13" s="2" t="n">
-        <v>73.75999999999999</v>
-      </c>
-      <c r="W13" t="n">
-        <v>57.52</v>
+        <v>68.18000000000001</v>
+      </c>
+      <c r="V13" t="n">
+        <v>21.77</v>
+      </c>
+      <c r="W13" s="2" t="n">
+        <v>79.61</v>
       </c>
       <c r="X13" t="n">
-        <v>64.73</v>
+        <v>18.9</v>
       </c>
       <c r="Y13" s="2" t="n">
-        <v>75.67</v>
+        <v>90.44</v>
       </c>
       <c r="Z13" t="n">
-        <v>62.54</v>
-      </c>
-      <c r="AA13" t="n">
-        <v>41.28</v>
+        <v>30.43</v>
+      </c>
+      <c r="AA13" s="2" t="n">
+        <v>87.83</v>
       </c>
       <c r="AB13" t="n">
-        <v>25.76</v>
-      </c>
-      <c r="AC13" s="2" t="n">
-        <v>83.02</v>
+        <v>5.78</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>10.05</v>
       </c>
       <c r="AD13" s="2" t="n">
-        <v>92.3</v>
+        <v>90.18000000000001</v>
       </c>
     </row>
     <row r="14">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Cyprus</t>
+          <t>Kosovo</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1831,90 +1831,90 @@
           <t>Lithuania</t>
         </is>
       </c>
-      <c r="D14" t="n">
-        <v>15.84</v>
+      <c r="D14" s="2" t="n">
+        <v>87.81</v>
       </c>
       <c r="E14" t="n">
-        <v>35.73</v>
+        <v>8.73</v>
       </c>
       <c r="F14" t="n">
-        <v>48.43</v>
+        <v>2.99</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
+          <t>3-0</t>
+        </is>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>96.54000000000001</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>90.8</v>
+      </c>
+      <c r="J14" t="n">
+        <v>11.72</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>86.62</v>
+      </c>
+      <c r="L14" t="n">
+        <v>68.54000000000001</v>
+      </c>
+      <c r="M14" t="n">
+        <v>52.38</v>
+      </c>
+      <c r="N14" s="2" t="n">
+        <v>71.41</v>
+      </c>
+      <c r="O14" t="n">
+        <v>35.17</v>
+      </c>
+      <c r="P14" t="n">
+        <v>49.47</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>49.58</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
           <t>0-0</t>
         </is>
       </c>
-      <c r="H14" t="n">
-        <v>51.56999999999999</v>
-      </c>
-      <c r="I14" t="n">
-        <v>64.27</v>
-      </c>
-      <c r="J14" s="2" t="n">
-        <v>84.16</v>
-      </c>
-      <c r="K14" t="n">
-        <v>35</v>
-      </c>
-      <c r="L14" t="n">
-        <v>13.6</v>
-      </c>
-      <c r="M14" s="2" t="n">
-        <v>95.98</v>
-      </c>
-      <c r="N14" s="2" t="n">
-        <v>99.03</v>
-      </c>
-      <c r="O14" t="n">
-        <v>17.07</v>
-      </c>
-      <c r="P14" t="n">
-        <v>17.76</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>62.47</v>
-      </c>
-      <c r="R14" t="n">
-        <v>19.75</v>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>0-0</t>
-        </is>
-      </c>
       <c r="T14" s="2" t="n">
-        <v>80.23</v>
+        <v>99.05</v>
       </c>
       <c r="U14" t="n">
-        <v>37.51000000000001</v>
-      </c>
-      <c r="V14" s="2" t="n">
-        <v>82.22</v>
+        <v>50.32</v>
+      </c>
+      <c r="V14" t="n">
+        <v>50.43</v>
       </c>
       <c r="W14" t="n">
-        <v>52</v>
+        <v>52.89</v>
       </c>
       <c r="X14" s="2" t="n">
-        <v>72.11</v>
-      </c>
-      <c r="Y14" t="n">
-        <v>30.85</v>
+        <v>80.47</v>
+      </c>
+      <c r="Y14" s="2" t="n">
+        <v>95.02</v>
       </c>
       <c r="Z14" t="n">
-        <v>59.38</v>
-      </c>
-      <c r="AA14" t="n">
-        <v>5.34</v>
+        <v>36.78</v>
+      </c>
+      <c r="AA14" s="2" t="n">
+        <v>81.04000000000001</v>
       </c>
       <c r="AB14" t="n">
-        <v>22.79</v>
-      </c>
-      <c r="AC14" s="2" t="n">
-        <v>99.36</v>
+        <v>7.83</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>40.15</v>
       </c>
       <c r="AD14" s="2" t="n">
-        <v>93.7</v>
+        <v>98.38</v>
       </c>
     </row>
     <row r="15">
@@ -1930,17 +1930,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Kosovo</t>
+          <t>Cyprus</t>
         </is>
       </c>
       <c r="D15" s="2" t="n">
-        <v>86.26000000000001</v>
+        <v>94.33</v>
       </c>
       <c r="E15" t="n">
-        <v>7.73</v>
+        <v>3.84</v>
       </c>
       <c r="F15" t="n">
-        <v>5.09</v>
+        <v>0.55</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1948,75 +1948,75 @@
         </is>
       </c>
       <c r="H15" s="2" t="n">
-        <v>93.99000000000001</v>
+        <v>98.17</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>91.35000000000001</v>
+        <v>94.88</v>
       </c>
       <c r="J15" t="n">
-        <v>12.82</v>
+        <v>4.39</v>
       </c>
       <c r="K15" s="2" t="n">
-        <v>90.86</v>
+        <v>88.33</v>
       </c>
       <c r="L15" s="2" t="n">
-        <v>78.25</v>
+        <v>72.47</v>
       </c>
       <c r="M15" t="n">
-        <v>39.27</v>
+        <v>46.52</v>
       </c>
       <c r="N15" t="n">
-        <v>58.7</v>
+        <v>66</v>
       </c>
       <c r="O15" t="n">
-        <v>50.48</v>
+        <v>15.7</v>
       </c>
       <c r="P15" t="n">
-        <v>25.12</v>
+        <v>69.16</v>
       </c>
       <c r="Q15" t="n">
-        <v>60.26</v>
+        <v>15.48</v>
       </c>
       <c r="R15" t="n">
-        <v>14.58</v>
+        <v>-0.68</v>
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>0-0</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="T15" s="2" t="n">
-        <v>85.38</v>
+        <v>84.64</v>
       </c>
       <c r="U15" t="n">
-        <v>39.7</v>
-      </c>
-      <c r="V15" s="2" t="n">
-        <v>74.84</v>
-      </c>
-      <c r="W15" t="n">
-        <v>56.19</v>
+        <v>68.47999999999999</v>
+      </c>
+      <c r="V15" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="W15" s="2" t="n">
+        <v>76.64</v>
       </c>
       <c r="X15" t="n">
-        <v>66.64</v>
+        <v>14.13</v>
       </c>
       <c r="Y15" s="2" t="n">
-        <v>95.93000000000001</v>
+        <v>96.14</v>
       </c>
       <c r="Z15" t="n">
-        <v>52.68</v>
+        <v>16.1</v>
       </c>
       <c r="AA15" s="2" t="n">
-        <v>85.02</v>
+        <v>86.73999999999999</v>
       </c>
       <c r="AB15" t="n">
-        <v>17.48</v>
+        <v>1.39</v>
       </c>
       <c r="AC15" t="n">
-        <v>32.91</v>
+        <v>29.18</v>
       </c>
       <c r="AD15" s="2" t="n">
-        <v>94.95999999999999</v>
+        <v>98.63</v>
       </c>
     </row>
     <row r="16">
@@ -2027,22 +2027,22 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Luxembourg</t>
+          <t>Bulgaria</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Bulgaria</t>
+          <t>Belarus</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>38.61</v>
+        <v>23.18</v>
       </c>
       <c r="E16" t="n">
-        <v>45.15</v>
+        <v>54.13</v>
       </c>
       <c r="F16" t="n">
-        <v>16.24</v>
+        <v>22.69</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -2050,28 +2050,28 @@
         </is>
       </c>
       <c r="H16" s="2" t="n">
-        <v>83.75999999999999</v>
+        <v>77.31</v>
       </c>
       <c r="I16" t="n">
-        <v>54.84999999999999</v>
-      </c>
-      <c r="J16" t="n">
-        <v>61.39</v>
+        <v>45.87</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>76.82000000000001</v>
       </c>
       <c r="K16" t="n">
-        <v>23.02</v>
+        <v>17.62</v>
       </c>
       <c r="L16" t="n">
-        <v>6.87</v>
+        <v>4.12</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>98.48</v>
+        <v>99.25</v>
       </c>
       <c r="N16" s="2" t="n">
-        <v>99.72</v>
+        <v>99.89</v>
       </c>
       <c r="O16" t="n">
-        <v>11.25</v>
+        <v>9.99</v>
       </c>
       <c r="P16" t="n">
         <v>0</v>
@@ -2103,22 +2103,22 @@
         <v>100</v>
       </c>
       <c r="Y16" t="n">
-        <v>46.81</v>
+        <v>31.68</v>
       </c>
       <c r="Z16" t="n">
-        <v>26.18</v>
+        <v>31.22</v>
       </c>
       <c r="AA16" t="n">
-        <v>13.23</v>
+        <v>5.65</v>
       </c>
       <c r="AB16" t="n">
-        <v>3.77</v>
+        <v>5.48</v>
       </c>
       <c r="AC16" s="2" t="n">
-        <v>97.37</v>
+        <v>99.31</v>
       </c>
       <c r="AD16" s="2" t="n">
-        <v>99.63</v>
+        <v>99.34</v>
       </c>
     </row>
     <row r="17">
@@ -2129,98 +2129,98 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>Luxembourg</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>Northern Ireland</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Belarus</t>
-        </is>
-      </c>
       <c r="D17" t="n">
-        <v>49.19</v>
+        <v>2.29</v>
       </c>
       <c r="E17" t="n">
-        <v>40.35</v>
-      </c>
-      <c r="F17" t="n">
-        <v>10.46</v>
+        <v>16.81</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>80.89</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>0-0</t>
-        </is>
-      </c>
-      <c r="H17" s="2" t="n">
-        <v>89.53999999999999</v>
-      </c>
-      <c r="I17" t="n">
-        <v>59.65</v>
-      </c>
-      <c r="J17" t="n">
-        <v>50.81</v>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>19.1</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>83.18000000000001</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>97.7</v>
       </c>
       <c r="K17" t="n">
-        <v>27.04</v>
+        <v>60.86</v>
       </c>
       <c r="L17" t="n">
-        <v>8.779999999999999</v>
+        <v>33.76</v>
       </c>
       <c r="M17" s="2" t="n">
-        <v>97.84999999999999</v>
+        <v>84.73</v>
       </c>
       <c r="N17" s="2" t="n">
-        <v>99.56999999999999</v>
+        <v>94.23999999999999</v>
       </c>
       <c r="O17" t="n">
-        <v>10.28</v>
+        <v>11.75</v>
       </c>
       <c r="P17" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="R17" t="n">
-        <v>0</v>
+        <v>-0</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>20.48</v>
+      </c>
+      <c r="R17" s="2" t="n">
+        <v>77.23</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>0-0</t>
-        </is>
-      </c>
-      <c r="T17" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="U17" t="n">
-        <v>0</v>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="T17" t="n">
+        <v>20.48</v>
+      </c>
+      <c r="U17" s="2" t="n">
+        <v>77.23</v>
       </c>
       <c r="V17" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="W17" t="n">
-        <v>0</v>
-      </c>
-      <c r="X17" s="2" t="n">
-        <v>100</v>
+        <v>97.71000000000001</v>
+      </c>
+      <c r="W17" s="2" t="n">
+        <v>77.23</v>
+      </c>
+      <c r="X17" t="n">
+        <v>52.96</v>
       </c>
       <c r="Y17" t="n">
-        <v>55.85</v>
-      </c>
-      <c r="Z17" t="n">
-        <v>19.94</v>
+        <v>13.74</v>
+      </c>
+      <c r="Z17" s="2" t="n">
+        <v>85.11</v>
       </c>
       <c r="AA17" t="n">
-        <v>19.75</v>
+        <v>0.99</v>
       </c>
       <c r="AB17" t="n">
-        <v>2.14</v>
+        <v>56.77</v>
       </c>
       <c r="AC17" s="2" t="n">
-        <v>95</v>
+        <v>99.94</v>
       </c>
       <c r="AD17" s="2" t="n">
-        <v>99.84</v>
+        <v>70.22</v>
       </c>
     </row>
     <row r="18">
@@ -2231,22 +2231,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>Liechtenstein</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>San Marino</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Gibraltar</t>
-        </is>
-      </c>
       <c r="D18" t="n">
-        <v>32</v>
+        <v>28.54</v>
       </c>
       <c r="E18" t="n">
-        <v>43.69</v>
+        <v>47.78</v>
       </c>
       <c r="F18" t="n">
-        <v>24.31</v>
+        <v>23.68</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -2254,28 +2254,28 @@
         </is>
       </c>
       <c r="H18" s="2" t="n">
-        <v>75.69</v>
+        <v>76.31999999999999</v>
       </c>
       <c r="I18" t="n">
-        <v>56.31</v>
-      </c>
-      <c r="J18" t="n">
-        <v>68</v>
+        <v>52.22</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>71.46000000000001</v>
       </c>
       <c r="K18" t="n">
-        <v>25.63</v>
+        <v>25.15</v>
       </c>
       <c r="L18" t="n">
-        <v>8.25</v>
+        <v>7.34</v>
       </c>
       <c r="M18" s="2" t="n">
-        <v>98.03</v>
+        <v>98.33</v>
       </c>
       <c r="N18" s="2" t="n">
-        <v>99.62</v>
+        <v>99.69</v>
       </c>
       <c r="O18" t="n">
-        <v>14.34</v>
+        <v>14.63</v>
       </c>
       <c r="P18" t="n">
         <v>0</v>
@@ -2307,22 +2307,22 @@
         <v>100</v>
       </c>
       <c r="Y18" t="n">
-        <v>43.06</v>
+        <v>40.35</v>
       </c>
       <c r="Z18" t="n">
-        <v>36.14</v>
+        <v>35.94</v>
       </c>
       <c r="AA18" t="n">
-        <v>10.99</v>
+        <v>9.529999999999999</v>
       </c>
       <c r="AB18" t="n">
-        <v>7.5</v>
+        <v>7.41</v>
       </c>
       <c r="AC18" s="2" t="n">
-        <v>98.04000000000001</v>
+        <v>98.43000000000001</v>
       </c>
       <c r="AD18" s="2" t="n">
-        <v>98.92</v>
+        <v>98.94</v>
       </c>
     </row>
     <row r="19">
@@ -2333,98 +2333,98 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Bosnia</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Bosnia</t>
-        </is>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>93.13</v>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>5.01</v>
       </c>
       <c r="E19" t="n">
-        <v>2.78</v>
-      </c>
-      <c r="F19" t="n">
-        <v>1.03</v>
+        <v>9.24</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>84.84</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>4-0</t>
-        </is>
-      </c>
-      <c r="H19" s="2" t="n">
-        <v>95.91</v>
+          <t>0-3</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>14.25</v>
       </c>
       <c r="I19" s="2" t="n">
-        <v>94.16</v>
-      </c>
-      <c r="J19" t="n">
-        <v>3.81</v>
+        <v>89.85000000000001</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>94.08</v>
       </c>
       <c r="K19" s="2" t="n">
-        <v>91.28</v>
+        <v>91.78</v>
       </c>
       <c r="L19" s="2" t="n">
-        <v>81.06</v>
+        <v>79</v>
       </c>
       <c r="M19" t="n">
-        <v>31.98</v>
+        <v>38.22</v>
       </c>
       <c r="N19" t="n">
-        <v>50.64</v>
+        <v>57.58</v>
       </c>
       <c r="O19" t="n">
-        <v>29</v>
-      </c>
-      <c r="P19" s="2" t="n">
-        <v>75.2</v>
+        <v>53.49</v>
+      </c>
+      <c r="P19" t="n">
+        <v>1.11</v>
       </c>
       <c r="Q19" t="n">
-        <v>17.63</v>
+        <v>31.41</v>
       </c>
       <c r="R19" t="n">
-        <v>-0.67</v>
+        <v>62.39</v>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>2-0</t>
-        </is>
-      </c>
-      <c r="T19" s="2" t="n">
-        <v>92.83</v>
-      </c>
-      <c r="U19" s="2" t="n">
-        <v>74.53</v>
-      </c>
-      <c r="V19" t="n">
-        <v>16.96</v>
+          <t>0-2</t>
+        </is>
+      </c>
+      <c r="T19" t="n">
+        <v>32.52</v>
+      </c>
+      <c r="U19" t="n">
+        <v>63.5</v>
+      </c>
+      <c r="V19" s="2" t="n">
+        <v>93.8</v>
       </c>
       <c r="W19" s="2" t="n">
-        <v>80.69</v>
+        <v>79.77</v>
       </c>
       <c r="X19" t="n">
-        <v>27.91</v>
-      </c>
-      <c r="Y19" s="2" t="n">
-        <v>95.54000000000001</v>
-      </c>
-      <c r="Z19" t="n">
-        <v>29.63</v>
-      </c>
-      <c r="AA19" s="2" t="n">
-        <v>89.58</v>
-      </c>
-      <c r="AB19" t="n">
-        <v>5.08</v>
-      </c>
-      <c r="AC19" t="n">
-        <v>20.1</v>
-      </c>
-      <c r="AD19" s="2" t="n">
-        <v>96.34</v>
+        <v>23.71</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>55.19</v>
+      </c>
+      <c r="Z19" s="2" t="n">
+        <v>95.93000000000001</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>19.45</v>
+      </c>
+      <c r="AB19" s="2" t="n">
+        <v>85.04000000000001</v>
+      </c>
+      <c r="AC19" s="2" t="n">
+        <v>94.18000000000001</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>32.87</v>
       </c>
     </row>
     <row r="20">
@@ -2435,98 +2435,98 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Hungary</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Hungary</t>
-        </is>
-      </c>
-      <c r="D20" s="2" t="n">
-        <v>81.98999999999999</v>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>3.13</v>
       </c>
       <c r="E20" t="n">
-        <v>11.73</v>
-      </c>
-      <c r="F20" t="n">
-        <v>6.17</v>
+        <v>13.29</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>83.51000000000001</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2-0</t>
-        </is>
-      </c>
-      <c r="H20" s="2" t="n">
-        <v>93.72</v>
+          <t>0-2</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>16.42</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>88.16</v>
-      </c>
-      <c r="J20" t="n">
-        <v>17.9</v>
+        <v>86.64</v>
+      </c>
+      <c r="J20" s="2" t="n">
+        <v>96.80000000000001</v>
       </c>
       <c r="K20" s="2" t="n">
-        <v>78.92</v>
+        <v>73.02</v>
       </c>
       <c r="L20" t="n">
-        <v>57.23</v>
-      </c>
-      <c r="M20" t="n">
-        <v>65.06</v>
+        <v>47.77</v>
+      </c>
+      <c r="M20" s="2" t="n">
+        <v>73.88</v>
       </c>
       <c r="N20" s="2" t="n">
-        <v>81.78</v>
+        <v>87.92</v>
       </c>
       <c r="O20" t="n">
-        <v>34.59</v>
+        <v>21.8</v>
       </c>
       <c r="P20" t="n">
-        <v>12.01</v>
+        <v>4.5</v>
       </c>
       <c r="Q20" t="n">
-        <v>64.12</v>
+        <v>61.11</v>
       </c>
       <c r="R20" t="n">
-        <v>23.86</v>
+        <v>34.36</v>
       </c>
       <c r="S20" t="inlineStr">
         <is>
           <t>0-0</t>
         </is>
       </c>
-      <c r="T20" s="2" t="n">
-        <v>76.13000000000001</v>
+      <c r="T20" t="n">
+        <v>65.61</v>
       </c>
       <c r="U20" t="n">
-        <v>35.87</v>
+        <v>38.86</v>
       </c>
       <c r="V20" s="2" t="n">
-        <v>87.98</v>
+        <v>95.47</v>
       </c>
       <c r="W20" t="n">
-        <v>46.75</v>
+        <v>45.28</v>
       </c>
       <c r="X20" s="2" t="n">
-        <v>78.97</v>
-      </c>
-      <c r="Y20" s="2" t="n">
-        <v>91.65000000000001</v>
-      </c>
-      <c r="Z20" t="n">
-        <v>38.6</v>
-      </c>
-      <c r="AA20" s="2" t="n">
-        <v>71.08</v>
+        <v>83.06999999999999</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>24.13</v>
+      </c>
+      <c r="Z20" s="2" t="n">
+        <v>90.02</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>3.18</v>
       </c>
       <c r="AB20" t="n">
-        <v>8.66</v>
-      </c>
-      <c r="AC20" t="n">
-        <v>54.47</v>
-      </c>
-      <c r="AD20" s="2" t="n">
-        <v>98.54000000000001</v>
+        <v>67.09999999999999</v>
+      </c>
+      <c r="AC20" s="2" t="n">
+        <v>99.65000000000001</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>59.32</v>
       </c>
     </row>
     <row r="21">
@@ -2537,7 +2537,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Albania</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -2546,51 +2546,51 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>64.8</v>
+        <v>34.89</v>
       </c>
       <c r="E21" t="n">
-        <v>21.49</v>
+        <v>41.4</v>
       </c>
       <c r="F21" t="n">
-        <v>13.7</v>
+        <v>23.71</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>0-0</t>
         </is>
       </c>
       <c r="H21" s="2" t="n">
-        <v>86.28999999999999</v>
-      </c>
-      <c r="I21" s="2" t="n">
-        <v>78.5</v>
+        <v>76.28999999999999</v>
+      </c>
+      <c r="I21" t="n">
+        <v>58.6</v>
       </c>
       <c r="J21" t="n">
-        <v>35.19</v>
+        <v>65.11</v>
       </c>
       <c r="K21" t="n">
-        <v>62.2</v>
+        <v>35</v>
       </c>
       <c r="L21" t="n">
-        <v>36.66</v>
+        <v>12.72</v>
       </c>
       <c r="M21" s="2" t="n">
-        <v>82.7</v>
+        <v>96.34999999999999</v>
       </c>
       <c r="N21" s="2" t="n">
-        <v>93.17</v>
+        <v>99.14</v>
       </c>
       <c r="O21" t="n">
-        <v>32.46</v>
+        <v>20.85</v>
       </c>
       <c r="P21" t="n">
-        <v>20.61</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="2" t="n">
-        <v>72.31999999999999</v>
+        <v>80.77</v>
       </c>
       <c r="R21" t="n">
-        <v>7.06</v>
+        <v>19.23</v>
       </c>
       <c r="S21" t="inlineStr">
         <is>
@@ -2598,37 +2598,37 @@
         </is>
       </c>
       <c r="T21" s="2" t="n">
-        <v>92.92999999999999</v>
+        <v>80.77</v>
       </c>
       <c r="U21" t="n">
-        <v>27.67</v>
+        <v>19.23</v>
       </c>
       <c r="V21" s="2" t="n">
-        <v>79.38</v>
+        <v>100</v>
       </c>
       <c r="W21" t="n">
-        <v>31.89</v>
+        <v>19.23</v>
       </c>
       <c r="X21" s="2" t="n">
-        <v>91.70999999999999</v>
-      </c>
-      <c r="Y21" s="2" t="n">
-        <v>80.04000000000001</v>
+        <v>98.02</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>50.56</v>
       </c>
       <c r="Z21" t="n">
-        <v>42.25</v>
+        <v>40.92</v>
       </c>
       <c r="AA21" t="n">
-        <v>47.87</v>
+        <v>15.73</v>
       </c>
       <c r="AB21" t="n">
-        <v>10.54</v>
+        <v>9.83</v>
       </c>
       <c r="AC21" s="2" t="n">
-        <v>78.04000000000001</v>
+        <v>96.53</v>
       </c>
       <c r="AD21" s="2" t="n">
-        <v>98.16</v>
+        <v>98.34999999999999</v>
       </c>
     </row>
     <row r="22">
@@ -2639,98 +2639,98 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Albania</t>
+          <t>Czechia</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Czechia</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>54.17</v>
+        <v>43.42</v>
       </c>
       <c r="E22" t="n">
-        <v>20.73</v>
+        <v>23.8</v>
       </c>
       <c r="F22" t="n">
-        <v>25.1</v>
+        <v>32.78</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>1-0</t>
-        </is>
-      </c>
-      <c r="H22" s="2" t="n">
-        <v>74.90000000000001</v>
+          <t>1-1</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>67.22</v>
       </c>
       <c r="I22" s="2" t="n">
-        <v>79.27000000000001</v>
+        <v>76.2</v>
       </c>
       <c r="J22" t="n">
-        <v>45.83</v>
+        <v>56.58</v>
       </c>
       <c r="K22" s="2" t="n">
-        <v>75.56999999999999</v>
+        <v>82.23</v>
       </c>
       <c r="L22" t="n">
-        <v>53.31</v>
+        <v>60.74</v>
       </c>
       <c r="M22" t="n">
-        <v>68.95</v>
+        <v>61.58</v>
       </c>
       <c r="N22" s="2" t="n">
-        <v>84.59</v>
+        <v>79.12</v>
       </c>
       <c r="O22" t="n">
-        <v>52.82</v>
+        <v>62.55</v>
       </c>
       <c r="P22" t="n">
-        <v>0</v>
+        <v>40.27</v>
       </c>
       <c r="Q22" t="n">
-        <v>62.33</v>
+        <v>56.78</v>
       </c>
       <c r="R22" t="n">
-        <v>37.66</v>
+        <v>2.9</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
           <t>0-0</t>
         </is>
       </c>
-      <c r="T22" t="n">
-        <v>62.33</v>
+      <c r="T22" s="2" t="n">
+        <v>97.05000000000001</v>
       </c>
       <c r="U22" t="n">
-        <v>37.66</v>
-      </c>
-      <c r="V22" s="2" t="n">
-        <v>99.98999999999999</v>
+        <v>43.17</v>
+      </c>
+      <c r="V22" t="n">
+        <v>59.68</v>
       </c>
       <c r="W22" t="n">
-        <v>37.66</v>
+        <v>48.73</v>
       </c>
       <c r="X22" s="2" t="n">
-        <v>91.79000000000001</v>
+        <v>81.31999999999999</v>
       </c>
       <c r="Y22" s="2" t="n">
-        <v>82.3</v>
-      </c>
-      <c r="Z22" t="n">
-        <v>66</v>
+        <v>81.61</v>
+      </c>
+      <c r="Z22" s="2" t="n">
+        <v>76.45</v>
       </c>
       <c r="AA22" t="n">
-        <v>51.66</v>
+        <v>50.48</v>
       </c>
       <c r="AB22" t="n">
-        <v>29.32</v>
+        <v>42.4</v>
       </c>
       <c r="AC22" s="2" t="n">
-        <v>74.87</v>
+        <v>75.88</v>
       </c>
       <c r="AD22" s="2" t="n">
-        <v>90.45999999999999</v>
+        <v>82.20999999999999</v>
       </c>
     </row>
     <row r="23">
@@ -2746,93 +2746,93 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Iceland</t>
+          <t>Turkiye</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>18.7</v>
+        <v>2.92</v>
       </c>
       <c r="E23" t="n">
-        <v>19.66</v>
+        <v>45.57</v>
       </c>
       <c r="F23" t="n">
-        <v>61.63</v>
+        <v>51.51</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>0-0</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>38.36</v>
-      </c>
-      <c r="I23" s="2" t="n">
-        <v>80.33</v>
+        <v>48.49</v>
+      </c>
+      <c r="I23" t="n">
+        <v>54.43</v>
       </c>
       <c r="J23" s="2" t="n">
-        <v>81.29000000000001</v>
-      </c>
-      <c r="K23" s="2" t="n">
-        <v>73.47</v>
+        <v>97.08</v>
+      </c>
+      <c r="K23" t="n">
+        <v>20.46</v>
       </c>
       <c r="L23" t="n">
-        <v>50.32</v>
+        <v>5.28</v>
       </c>
       <c r="M23" s="2" t="n">
-        <v>71.68000000000001</v>
+        <v>98.95</v>
       </c>
       <c r="N23" s="2" t="n">
-        <v>86.47</v>
+        <v>99.83</v>
       </c>
       <c r="O23" t="n">
-        <v>46.98</v>
+        <v>3.38</v>
       </c>
       <c r="P23" t="n">
         <v>0</v>
       </c>
-      <c r="Q23" t="n">
-        <v>28.09</v>
-      </c>
-      <c r="R23" s="2" t="n">
-        <v>70.94</v>
+      <c r="Q23" s="2" t="n">
+        <v>90.14</v>
+      </c>
+      <c r="R23" t="n">
+        <v>9.859999999999999</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>0-1</t>
-        </is>
-      </c>
-      <c r="T23" t="n">
-        <v>28.09</v>
-      </c>
-      <c r="U23" s="2" t="n">
-        <v>70.94</v>
+          <t>0-0</t>
+        </is>
+      </c>
+      <c r="T23" s="2" t="n">
+        <v>90.14</v>
+      </c>
+      <c r="U23" t="n">
+        <v>9.859999999999999</v>
       </c>
       <c r="V23" s="2" t="n">
-        <v>99.03</v>
-      </c>
-      <c r="W23" s="2" t="n">
-        <v>70.94</v>
-      </c>
-      <c r="X23" t="n">
-        <v>63.75</v>
+        <v>100</v>
+      </c>
+      <c r="W23" t="n">
+        <v>9.859999999999999</v>
+      </c>
+      <c r="X23" s="2" t="n">
+        <v>99.5</v>
       </c>
       <c r="Y23" t="n">
-        <v>57.7</v>
-      </c>
-      <c r="Z23" s="2" t="n">
-        <v>83.90000000000001</v>
+        <v>6.23</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>53.79</v>
       </c>
       <c r="AA23" t="n">
-        <v>21.31</v>
+        <v>0.2</v>
       </c>
       <c r="AB23" t="n">
-        <v>54.51</v>
+        <v>18.12</v>
       </c>
       <c r="AC23" s="2" t="n">
-        <v>94.34</v>
+        <v>100</v>
       </c>
       <c r="AD23" s="2" t="n">
-        <v>72.33</v>
+        <v>95.65000000000001</v>
       </c>
     </row>
     <row r="24">
@@ -2843,98 +2843,98 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Turkiye</t>
+          <t>Wales</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Wales</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>48.11</v>
+          <t>Iceland</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>76.81</v>
       </c>
       <c r="E24" t="n">
-        <v>35</v>
+        <v>12.33</v>
       </c>
       <c r="F24" t="n">
-        <v>16.89</v>
+        <v>10.09</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="H24" s="2" t="n">
-        <v>83.11</v>
-      </c>
-      <c r="I24" t="n">
-        <v>65</v>
+        <v>89.14</v>
+      </c>
+      <c r="I24" s="2" t="n">
+        <v>86.90000000000001</v>
       </c>
       <c r="J24" t="n">
-        <v>51.89</v>
-      </c>
-      <c r="K24" t="n">
-        <v>36.5</v>
-      </c>
-      <c r="L24" t="n">
-        <v>14.61</v>
-      </c>
-      <c r="M24" s="2" t="n">
-        <v>95.55</v>
-      </c>
-      <c r="N24" s="2" t="n">
-        <v>98.89</v>
+        <v>22.42</v>
+      </c>
+      <c r="K24" s="2" t="n">
+        <v>93.68000000000001</v>
+      </c>
+      <c r="L24" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="M24" t="n">
+        <v>32.51</v>
+      </c>
+      <c r="N24" t="n">
+        <v>51.26</v>
       </c>
       <c r="O24" t="n">
-        <v>18.42</v>
-      </c>
-      <c r="P24" t="n">
-        <v>0</v>
+        <v>68.19</v>
+      </c>
+      <c r="P24" s="2" t="n">
+        <v>79.67</v>
       </c>
       <c r="Q24" t="n">
-        <v>61.91</v>
+        <v>6.81</v>
       </c>
       <c r="R24" t="n">
-        <v>38.07</v>
+        <v>-0</v>
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>0-0</t>
-        </is>
-      </c>
-      <c r="T24" t="n">
-        <v>61.91</v>
-      </c>
-      <c r="U24" t="n">
-        <v>38.07</v>
-      </c>
-      <c r="V24" s="2" t="n">
-        <v>99.97999999999999</v>
-      </c>
-      <c r="W24" t="n">
-        <v>38.07</v>
-      </c>
-      <c r="X24" s="2" t="n">
-        <v>91.59999999999999</v>
-      </c>
-      <c r="Y24" t="n">
-        <v>59.93</v>
-      </c>
-      <c r="Z24" t="n">
-        <v>32.92</v>
-      </c>
-      <c r="AA24" t="n">
-        <v>23.29</v>
+          <t>2-0</t>
+        </is>
+      </c>
+      <c r="T24" s="2" t="n">
+        <v>86.48</v>
+      </c>
+      <c r="U24" s="2" t="n">
+        <v>79.67</v>
+      </c>
+      <c r="V24" t="n">
+        <v>6.81</v>
+      </c>
+      <c r="W24" s="2" t="n">
+        <v>79.67</v>
+      </c>
+      <c r="X24" t="n">
+        <v>25.09</v>
+      </c>
+      <c r="Y24" s="2" t="n">
+        <v>95.76000000000001</v>
+      </c>
+      <c r="Z24" s="2" t="n">
+        <v>70.59999999999999</v>
+      </c>
+      <c r="AA24" s="2" t="n">
+        <v>84.09</v>
       </c>
       <c r="AB24" t="n">
-        <v>6.14</v>
-      </c>
-      <c r="AC24" s="2" t="n">
-        <v>93.47</v>
+        <v>35.01</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>34.74</v>
       </c>
       <c r="AD24" s="2" t="n">
-        <v>99.20999999999999</v>
+        <v>86.33</v>
       </c>
     </row>
     <row r="25">
@@ -2945,7 +2945,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Azerbaijan</t>
+          <t>Slovakia</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -2953,52 +2953,52 @@
           <t>Estonia</t>
         </is>
       </c>
-      <c r="D25" t="n">
-        <v>45.37</v>
+      <c r="D25" s="2" t="n">
+        <v>73.98999999999999</v>
       </c>
       <c r="E25" t="n">
-        <v>23.75</v>
+        <v>20.72</v>
       </c>
       <c r="F25" t="n">
-        <v>30.87</v>
+        <v>5.28</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
           <t>1-0</t>
         </is>
       </c>
-      <c r="H25" t="n">
-        <v>69.12</v>
+      <c r="H25" s="2" t="n">
+        <v>94.70999999999999</v>
       </c>
       <c r="I25" s="2" t="n">
-        <v>76.23999999999999</v>
+        <v>79.27</v>
       </c>
       <c r="J25" t="n">
-        <v>54.62</v>
+        <v>26</v>
       </c>
       <c r="K25" t="n">
-        <v>67.73999999999999</v>
+        <v>60.13</v>
       </c>
       <c r="L25" t="n">
-        <v>43.39</v>
+        <v>32.97</v>
       </c>
       <c r="M25" s="2" t="n">
-        <v>77.58</v>
+        <v>85.28</v>
       </c>
       <c r="N25" s="2" t="n">
-        <v>90.23999999999999</v>
+        <v>94.52</v>
       </c>
       <c r="O25" t="n">
-        <v>46.73</v>
+        <v>20.32</v>
       </c>
       <c r="P25" t="n">
-        <v>26.67</v>
+        <v>57.58</v>
       </c>
       <c r="Q25" t="n">
-        <v>53.61</v>
+        <v>36.05</v>
       </c>
       <c r="R25" t="n">
-        <v>19.25</v>
+        <v>2.59</v>
       </c>
       <c r="S25" t="inlineStr">
         <is>
@@ -3006,37 +3006,37 @@
         </is>
       </c>
       <c r="T25" s="2" t="n">
-        <v>80.28</v>
+        <v>93.63</v>
       </c>
       <c r="U25" t="n">
-        <v>45.92</v>
-      </c>
-      <c r="V25" s="2" t="n">
-        <v>72.86</v>
+        <v>60.17</v>
+      </c>
+      <c r="V25" t="n">
+        <v>38.64</v>
       </c>
       <c r="W25" s="2" t="n">
-        <v>72.36</v>
+        <v>79.2</v>
       </c>
       <c r="X25" t="n">
-        <v>36.57</v>
+        <v>24.71</v>
       </c>
       <c r="Y25" s="2" t="n">
-        <v>74.27</v>
+        <v>82.48999999999999</v>
       </c>
       <c r="Z25" t="n">
-        <v>65.23</v>
+        <v>24.51</v>
       </c>
       <c r="AA25" t="n">
-        <v>39.34</v>
+        <v>51.98</v>
       </c>
       <c r="AB25" t="n">
-        <v>28.5</v>
+        <v>3.29</v>
       </c>
       <c r="AC25" s="2" t="n">
-        <v>84.37</v>
+        <v>74.59</v>
       </c>
       <c r="AD25" s="2" t="n">
-        <v>90.90000000000001</v>
+        <v>99.69</v>
       </c>
     </row>
     <row r="26">
@@ -3052,55 +3052,55 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Slovakia</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>65.23999999999999</v>
+          <t>Azerbaijan</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>86.84</v>
       </c>
       <c r="E26" t="n">
-        <v>18.54</v>
+        <v>1.44</v>
       </c>
       <c r="F26" t="n">
-        <v>16.2</v>
+        <v>0.41</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>5-0</t>
         </is>
       </c>
       <c r="H26" s="2" t="n">
-        <v>83.78</v>
+        <v>88.28</v>
       </c>
       <c r="I26" s="2" t="n">
-        <v>81.44</v>
+        <v>87.25</v>
       </c>
       <c r="J26" t="n">
-        <v>34.73999999999999</v>
+        <v>1.85</v>
       </c>
       <c r="K26" s="2" t="n">
-        <v>74.33</v>
-      </c>
-      <c r="L26" t="n">
-        <v>51.38</v>
-      </c>
-      <c r="M26" s="2" t="n">
-        <v>70.72</v>
-      </c>
-      <c r="N26" s="2" t="n">
-        <v>85.81999999999999</v>
+        <v>87.06</v>
+      </c>
+      <c r="L26" s="2" t="n">
+        <v>82.78</v>
+      </c>
+      <c r="M26" t="n">
+        <v>14.53</v>
+      </c>
+      <c r="N26" t="n">
+        <v>27.61</v>
       </c>
       <c r="O26" t="n">
-        <v>45.79</v>
+        <v>33.72</v>
       </c>
       <c r="P26" t="n">
-        <v>62.89</v>
+        <v>69.11</v>
       </c>
       <c r="Q26" t="n">
-        <v>33.03</v>
+        <v>27.37</v>
       </c>
       <c r="R26" t="n">
-        <v>0.97</v>
+        <v>-0.32</v>
       </c>
       <c r="S26" t="inlineStr">
         <is>
@@ -3108,37 +3108,37 @@
         </is>
       </c>
       <c r="T26" s="2" t="n">
-        <v>95.92</v>
+        <v>96.48</v>
       </c>
       <c r="U26" t="n">
-        <v>63.86</v>
+        <v>68.79000000000001</v>
       </c>
       <c r="V26" t="n">
-        <v>34</v>
+        <v>27.05</v>
       </c>
       <c r="W26" s="2" t="n">
-        <v>78.40000000000001</v>
+        <v>79.05</v>
       </c>
       <c r="X26" t="n">
-        <v>33.01</v>
+        <v>34.78</v>
       </c>
       <c r="Y26" s="2" t="n">
-        <v>85.45</v>
+        <v>88.31</v>
       </c>
       <c r="Z26" t="n">
-        <v>55.15</v>
-      </c>
-      <c r="AA26" t="n">
-        <v>57.43</v>
+        <v>33.85</v>
+      </c>
+      <c r="AA26" s="2" t="n">
+        <v>86.22</v>
       </c>
       <c r="AB26" t="n">
-        <v>19.19</v>
+        <v>7.49</v>
       </c>
       <c r="AC26" t="n">
-        <v>69.59</v>
+        <v>8.31</v>
       </c>
       <c r="AD26" s="2" t="n">
-        <v>95.20999999999999</v>
+        <v>87.53</v>
       </c>
     </row>
     <row r="27">
@@ -3149,98 +3149,98 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>Malta</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
           <t>Andorra</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Moldova</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
+      <c r="D27" s="2" t="n">
+        <v>75.62</v>
+      </c>
+      <c r="E27" t="n">
+        <v>24.38</v>
+      </c>
+      <c r="F27" t="n">
         <v>0</v>
       </c>
-      <c r="E27" t="n">
-        <v>26.31</v>
-      </c>
-      <c r="F27" s="2" t="n">
-        <v>73.69</v>
-      </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>0-1</t>
-        </is>
-      </c>
-      <c r="H27" t="n">
-        <v>26.31</v>
+          <t>1-0</t>
+        </is>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>100</v>
       </c>
       <c r="I27" s="2" t="n">
-        <v>73.69</v>
-      </c>
-      <c r="J27" s="2" t="n">
-        <v>100</v>
+        <v>75.62</v>
+      </c>
+      <c r="J27" t="n">
+        <v>24.38</v>
       </c>
       <c r="K27" t="n">
-        <v>38.56</v>
+        <v>41.21</v>
       </c>
       <c r="L27" t="n">
-        <v>15.11</v>
+        <v>16.92</v>
       </c>
       <c r="M27" s="2" t="n">
-        <v>95.33</v>
+        <v>94.5</v>
       </c>
       <c r="N27" s="2" t="n">
-        <v>98.81</v>
+        <v>98.53</v>
       </c>
       <c r="O27" t="n">
         <v>0</v>
       </c>
-      <c r="P27" t="n">
+      <c r="P27" s="2" t="n">
+        <v>70.73</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>28.33</v>
+      </c>
+      <c r="R27" t="n">
+        <v>-0</v>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>1-0</t>
+        </is>
+      </c>
+      <c r="T27" s="2" t="n">
+        <v>99.06</v>
+      </c>
+      <c r="U27" s="2" t="n">
+        <v>70.73</v>
+      </c>
+      <c r="V27" t="n">
+        <v>28.33</v>
+      </c>
+      <c r="W27" s="2" t="n">
+        <v>70.73</v>
+      </c>
+      <c r="X27" t="n">
+        <v>64.06</v>
+      </c>
+      <c r="Y27" s="2" t="n">
+        <v>75.62</v>
+      </c>
+      <c r="Z27" t="n">
         <v>0</v>
       </c>
-      <c r="Q27" t="n">
-        <v>45.36</v>
-      </c>
-      <c r="R27" t="n">
-        <v>54.5</v>
-      </c>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>0-0</t>
-        </is>
-      </c>
-      <c r="T27" t="n">
-        <v>45.36</v>
-      </c>
-      <c r="U27" t="n">
-        <v>54.5</v>
-      </c>
-      <c r="V27" s="2" t="n">
-        <v>99.86</v>
-      </c>
-      <c r="W27" t="n">
-        <v>54.5</v>
-      </c>
-      <c r="X27" s="2" t="n">
-        <v>81.22</v>
-      </c>
-      <c r="Y27" t="n">
+      <c r="AA27" t="n">
+        <v>41.21</v>
+      </c>
+      <c r="AB27" t="n">
         <v>0</v>
       </c>
-      <c r="Z27" s="2" t="n">
-        <v>73.69</v>
-      </c>
-      <c r="AA27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB27" t="n">
-        <v>38.56</v>
-      </c>
       <c r="AC27" s="2" t="n">
+        <v>83.08</v>
+      </c>
+      <c r="AD27" s="2" t="n">
         <v>100</v>
-      </c>
-      <c r="AD27" s="2" t="n">
-        <v>84.89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
need to add article betting strategy to comparer & updated until 04.03.2025
</commit_message>
<xml_diff>
--- a/UEFA.xlsx
+++ b/UEFA.xlsx
@@ -599,98 +599,98 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Milan</t>
+          <t>Club Brugge</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Feyenoord</t>
+          <t>Aston Villa</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>63.16</v>
+        <v>32.44</v>
       </c>
       <c r="E2" t="n">
-        <v>14.51</v>
+        <v>26.08</v>
       </c>
       <c r="F2" t="n">
-        <v>22.23</v>
+        <v>41.48</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2-1</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>77.67</v>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>58.52</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>85.39</v>
+        <v>73.91999999999999</v>
       </c>
       <c r="J2" t="n">
-        <v>36.74</v>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>86.83</v>
-      </c>
-      <c r="L2" s="2" t="n">
-        <v>72.56999999999999</v>
-      </c>
-      <c r="M2" t="n">
-        <v>47.91</v>
-      </c>
-      <c r="N2" t="n">
-        <v>67.31</v>
+        <v>67.56</v>
+      </c>
+      <c r="K2" t="n">
+        <v>63.83</v>
+      </c>
+      <c r="L2" t="n">
+        <v>38.43</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>81.41</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>92.45999999999999</v>
       </c>
       <c r="O2" t="n">
-        <v>65.31</v>
+        <v>43.47</v>
       </c>
       <c r="P2" t="n">
-        <v>39.28</v>
+        <v>55.21</v>
       </c>
       <c r="Q2" t="n">
-        <v>20.63</v>
+        <v>32.22</v>
       </c>
       <c r="R2" t="n">
-        <v>38.34</v>
+        <v>12.17</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
           <t>1-0</t>
         </is>
       </c>
-      <c r="T2" t="n">
-        <v>59.91</v>
-      </c>
-      <c r="U2" s="2" t="n">
-        <v>77.62</v>
+      <c r="T2" s="2" t="n">
+        <v>87.43000000000001</v>
+      </c>
+      <c r="U2" t="n">
+        <v>67.38</v>
       </c>
       <c r="V2" t="n">
-        <v>58.97</v>
+        <v>44.39</v>
       </c>
       <c r="W2" s="2" t="n">
-        <v>93.09</v>
+        <v>74.37</v>
       </c>
       <c r="X2" t="n">
-        <v>32.56</v>
-      </c>
-      <c r="Y2" s="2" t="n">
-        <v>91.05</v>
-      </c>
-      <c r="Z2" s="2" t="n">
-        <v>73.97</v>
+        <v>63.89</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>64.04000000000001</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>69.98999999999999</v>
       </c>
       <c r="AA2" t="n">
-        <v>69.58</v>
+        <v>27.26</v>
       </c>
       <c r="AB2" t="n">
-        <v>38.99</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>56.34</v>
+        <v>33.87</v>
+      </c>
+      <c r="AC2" s="2" t="n">
+        <v>91.55</v>
       </c>
       <c r="AD2" s="2" t="n">
-        <v>84.5</v>
+        <v>87.87</v>
       </c>
     </row>
     <row r="3">
@@ -701,98 +701,98 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Atalanta</t>
+          <t>Dortmund</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Club Brugge</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>77.93000000000001</v>
+          <t>Lille</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>52.02</v>
       </c>
       <c r="E3" t="n">
-        <v>12.41</v>
+        <v>18.16</v>
       </c>
       <c r="F3" t="n">
-        <v>9.619999999999999</v>
+        <v>29.73</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>2-1</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>70.18000000000001</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>81.75</v>
+      </c>
+      <c r="J3" t="n">
+        <v>47.89</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>91.23999999999999</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>78.45999999999999</v>
+      </c>
+      <c r="M3" t="n">
+        <v>40.13</v>
+      </c>
+      <c r="N3" t="n">
+        <v>59.6</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>74.8</v>
+      </c>
+      <c r="P3" t="n">
+        <v>64.61</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>30</v>
+      </c>
+      <c r="R3" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
           <t>1-0</t>
         </is>
       </c>
-      <c r="H3" s="2" t="n">
-        <v>90.34</v>
-      </c>
-      <c r="I3" s="2" t="n">
-        <v>87.55000000000001</v>
-      </c>
-      <c r="J3" t="n">
-        <v>22.03</v>
-      </c>
-      <c r="K3" s="2" t="n">
-        <v>73.48999999999999</v>
-      </c>
-      <c r="L3" t="n">
-        <v>51.32</v>
-      </c>
-      <c r="M3" s="2" t="n">
-        <v>70.75</v>
-      </c>
-      <c r="N3" s="2" t="n">
-        <v>85.84999999999999</v>
-      </c>
-      <c r="O3" t="n">
-        <v>34.46</v>
-      </c>
-      <c r="P3" t="n">
-        <v>29.63</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>52.19</v>
-      </c>
-      <c r="R3" t="n">
-        <v>18.17</v>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>0-0</t>
-        </is>
-      </c>
       <c r="T3" s="2" t="n">
-        <v>81.81999999999999</v>
+        <v>94.61</v>
       </c>
       <c r="U3" t="n">
-        <v>47.8</v>
-      </c>
-      <c r="V3" s="2" t="n">
-        <v>70.36</v>
-      </c>
-      <c r="W3" t="n">
-        <v>52.4</v>
-      </c>
-      <c r="X3" s="2" t="n">
-        <v>85.52</v>
+        <v>69.31</v>
+      </c>
+      <c r="V3" t="n">
+        <v>34.7</v>
+      </c>
+      <c r="W3" s="2" t="n">
+        <v>72.59</v>
+      </c>
+      <c r="X3" t="n">
+        <v>63.87</v>
       </c>
       <c r="Y3" s="2" t="n">
-        <v>88.86</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>41.15</v>
+        <v>90.68000000000001</v>
+      </c>
+      <c r="Z3" s="2" t="n">
+        <v>83.15000000000001</v>
       </c>
       <c r="AA3" t="n">
-        <v>64.48</v>
+        <v>68.69</v>
       </c>
       <c r="AB3" t="n">
-        <v>9.949999999999999</v>
+        <v>53.23</v>
       </c>
       <c r="AC3" t="n">
-        <v>62.29</v>
+        <v>57.41</v>
       </c>
       <c r="AD3" s="2" t="n">
-        <v>98.27</v>
+        <v>73.39</v>
       </c>
     </row>
     <row r="4">
@@ -803,98 +803,98 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Benfica</t>
+          <t>PSV</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Monaco</t>
+          <t>Arsenal</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>61.79</v>
+        <v>10.89</v>
       </c>
       <c r="E4" t="n">
-        <v>15.35</v>
-      </c>
-      <c r="F4" t="n">
-        <v>22.82</v>
+        <v>16.06</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>73.01000000000001</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1-0</t>
-        </is>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>77.14</v>
+          <t>0-2</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>26.95</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>84.61</v>
-      </c>
-      <c r="J4" t="n">
-        <v>38.17</v>
+        <v>83.90000000000001</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>89.07000000000001</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>81.43000000000001</v>
+        <v>77.17</v>
       </c>
       <c r="L4" t="n">
-        <v>63.86</v>
+        <v>54.68</v>
       </c>
       <c r="M4" t="n">
-        <v>58.21</v>
+        <v>67.61</v>
       </c>
       <c r="N4" s="2" t="n">
-        <v>76.40000000000001</v>
+        <v>83.65000000000001</v>
       </c>
       <c r="O4" t="n">
-        <v>58.06</v>
+        <v>42.81</v>
       </c>
       <c r="P4" t="n">
-        <v>43.65</v>
+        <v>8.779999999999999</v>
       </c>
       <c r="Q4" t="n">
-        <v>36.7</v>
-      </c>
-      <c r="R4" t="n">
-        <v>19.53</v>
+        <v>13.25</v>
+      </c>
+      <c r="R4" s="2" t="n">
+        <v>70.43000000000001</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>0-0</t>
-        </is>
-      </c>
-      <c r="T4" s="2" t="n">
-        <v>80.34999999999999</v>
-      </c>
-      <c r="U4" t="n">
-        <v>63.18</v>
-      </c>
-      <c r="V4" t="n">
-        <v>56.23</v>
+          <t>0-2</t>
+        </is>
+      </c>
+      <c r="T4" t="n">
+        <v>22.03</v>
+      </c>
+      <c r="U4" s="2" t="n">
+        <v>79.21000000000001</v>
+      </c>
+      <c r="V4" s="2" t="n">
+        <v>83.68000000000001</v>
       </c>
       <c r="W4" s="2" t="n">
-        <v>70.94</v>
-      </c>
-      <c r="X4" s="2" t="n">
-        <v>70.06999999999999</v>
-      </c>
-      <c r="Y4" s="2" t="n">
-        <v>88.01000000000001</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>68.88</v>
+        <v>87.62</v>
+      </c>
+      <c r="X4" t="n">
+        <v>25.53</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>49.14</v>
+      </c>
+      <c r="Z4" s="2" t="n">
+        <v>88.81</v>
       </c>
       <c r="AA4" t="n">
-        <v>62.62</v>
+        <v>14.76</v>
       </c>
       <c r="AB4" t="n">
-        <v>32.57</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>64.31</v>
-      </c>
-      <c r="AD4" s="2" t="n">
-        <v>88.59999999999999</v>
+        <v>64.36</v>
+      </c>
+      <c r="AC4" s="2" t="n">
+        <v>96.81999999999999</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>62.42</v>
       </c>
     </row>
     <row r="5">
@@ -905,98 +905,98 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Bayern</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Celtic</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>73.88</v>
+          <t>Athletico Madrid</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>64.64</v>
       </c>
       <c r="E5" t="n">
-        <v>12.36</v>
+        <v>16.14</v>
       </c>
       <c r="F5" t="n">
-        <v>13.66</v>
+        <v>19.06</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="H5" s="2" t="n">
-        <v>86.23999999999999</v>
+        <v>80.78</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>87.53999999999999</v>
+        <v>83.7</v>
       </c>
       <c r="J5" t="n">
-        <v>26.02</v>
+        <v>35.2</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>81.7</v>
-      </c>
-      <c r="L5" t="n">
-        <v>63.7</v>
+        <v>89.88</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>75.77</v>
       </c>
       <c r="M5" t="n">
-        <v>58.33</v>
-      </c>
-      <c r="N5" s="2" t="n">
-        <v>76.5</v>
+        <v>43.69</v>
+      </c>
+      <c r="N5" t="n">
+        <v>63.23</v>
       </c>
       <c r="O5" t="n">
-        <v>50.46</v>
+        <v>68.31999999999999</v>
       </c>
       <c r="P5" t="n">
-        <v>61.12</v>
+        <v>24.38</v>
       </c>
       <c r="Q5" t="n">
-        <v>22.66</v>
+        <v>30.93</v>
       </c>
       <c r="R5" t="n">
-        <v>14.88</v>
+        <v>44.39</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>1-0</t>
-        </is>
-      </c>
-      <c r="T5" s="2" t="n">
-        <v>83.78</v>
-      </c>
-      <c r="U5" s="2" t="n">
-        <v>76</v>
-      </c>
-      <c r="V5" t="n">
-        <v>37.54</v>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="T5" t="n">
+        <v>55.31</v>
+      </c>
+      <c r="U5" t="n">
+        <v>68.77</v>
+      </c>
+      <c r="V5" s="2" t="n">
+        <v>75.31999999999999</v>
       </c>
       <c r="W5" s="2" t="n">
-        <v>85.23999999999999</v>
+        <v>79.87</v>
       </c>
       <c r="X5" t="n">
-        <v>47.84</v>
+        <v>58.23</v>
       </c>
       <c r="Y5" s="2" t="n">
-        <v>91.05</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>57.77</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>69.56999999999999</v>
+        <v>92.51000000000001</v>
+      </c>
+      <c r="Z5" s="2" t="n">
+        <v>74.47</v>
+      </c>
+      <c r="AA5" s="2" t="n">
+        <v>73.34999999999999</v>
       </c>
       <c r="AB5" t="n">
-        <v>21.39</v>
+        <v>39.71</v>
       </c>
       <c r="AC5" t="n">
-        <v>56.36</v>
+        <v>51.53</v>
       </c>
       <c r="AD5" s="2" t="n">
-        <v>94.22</v>
+        <v>83.95</v>
       </c>
     </row>
     <row r="6">
@@ -1007,98 +1007,98 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>Feyenoord</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Sporting</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>77.40000000000001</v>
+          <t>Inter</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>4.82</v>
       </c>
       <c r="E6" t="n">
-        <v>10.16</v>
-      </c>
-      <c r="F6" t="n">
-        <v>11.79</v>
+        <v>24.17</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>71</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3-1</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>87.56</v>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>28.99</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>89.19</v>
-      </c>
-      <c r="J6" t="n">
-        <v>21.95</v>
-      </c>
-      <c r="K6" s="2" t="n">
-        <v>91.98</v>
-      </c>
-      <c r="L6" s="2" t="n">
-        <v>81.97</v>
-      </c>
-      <c r="M6" t="n">
-        <v>34.26</v>
-      </c>
-      <c r="N6" t="n">
-        <v>53.25</v>
+        <v>75.81999999999999</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>95.17</v>
+      </c>
+      <c r="K6" t="n">
+        <v>47.59</v>
+      </c>
+      <c r="L6" t="n">
+        <v>22.14</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>91.86</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>97.53</v>
       </c>
       <c r="O6" t="n">
-        <v>66.29000000000001</v>
-      </c>
-      <c r="P6" s="2" t="n">
-        <v>70.77</v>
+        <v>11.83</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>24.52</v>
+        <v>36.99</v>
       </c>
       <c r="R6" t="n">
-        <v>3.37</v>
+        <v>62.65</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>1-0</t>
-        </is>
-      </c>
-      <c r="T6" s="2" t="n">
-        <v>95.28999999999999</v>
-      </c>
-      <c r="U6" s="2" t="n">
-        <v>74.14</v>
-      </c>
-      <c r="V6" t="n">
-        <v>27.89</v>
-      </c>
-      <c r="W6" s="2" t="n">
-        <v>76.59999999999999</v>
-      </c>
-      <c r="X6" t="n">
-        <v>57.4</v>
-      </c>
-      <c r="Y6" s="2" t="n">
-        <v>95.55</v>
+          <t>0-0</t>
+        </is>
+      </c>
+      <c r="T6" t="n">
+        <v>36.99</v>
+      </c>
+      <c r="U6" t="n">
+        <v>62.65</v>
+      </c>
+      <c r="V6" s="2" t="n">
+        <v>99.64</v>
+      </c>
+      <c r="W6" t="n">
+        <v>62.65</v>
+      </c>
+      <c r="X6" s="2" t="n">
+        <v>73.78</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>16.16</v>
       </c>
       <c r="Z6" s="2" t="n">
-        <v>70.22</v>
-      </c>
-      <c r="AA6" s="2" t="n">
-        <v>83.13</v>
+        <v>76.34999999999999</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>1.38</v>
       </c>
       <c r="AB6" t="n">
-        <v>34.49</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>36.53</v>
+        <v>42.26</v>
+      </c>
+      <c r="AC6" s="2" t="n">
+        <v>99.92</v>
       </c>
       <c r="AD6" s="2" t="n">
-        <v>86.78</v>
+        <v>82.31999999999999</v>
       </c>
     </row>
     <row r="7">
@@ -1109,98 +1109,98 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>PSV</t>
+          <t>Benfica</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Juventus</t>
+          <t>Barcelona</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>42.6</v>
+        <v>38.14</v>
       </c>
       <c r="E7" t="n">
-        <v>21.16</v>
+        <v>18.23</v>
       </c>
       <c r="F7" t="n">
-        <v>36.24</v>
+        <v>43.51</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
+          <t>2-2</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>56.37</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>81.65000000000001</v>
+      </c>
+      <c r="J7" t="n">
+        <v>61.73999999999999</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>93.23</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>82.56999999999999</v>
+      </c>
+      <c r="M7" t="n">
+        <v>34.16</v>
+      </c>
+      <c r="N7" t="n">
+        <v>53.13</v>
+      </c>
+      <c r="O7" s="2" t="n">
+        <v>79.34</v>
+      </c>
+      <c r="P7" t="n">
+        <v>40.65</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>27.64</v>
+      </c>
+      <c r="R7" t="n">
+        <v>31.26</v>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
           <t>1-0</t>
         </is>
       </c>
-      <c r="H7" t="n">
-        <v>63.76000000000001</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <v>78.84</v>
-      </c>
-      <c r="J7" t="n">
-        <v>57.40000000000001</v>
-      </c>
-      <c r="K7" t="n">
-        <v>62.29</v>
-      </c>
-      <c r="L7" t="n">
-        <v>39.35</v>
-      </c>
-      <c r="M7" s="2" t="n">
-        <v>80.73</v>
-      </c>
-      <c r="N7" s="2" t="n">
-        <v>92.08</v>
-      </c>
-      <c r="O7" t="n">
-        <v>42</v>
-      </c>
-      <c r="P7" t="n">
-        <v>31.79</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>41.91</v>
-      </c>
-      <c r="R7" t="n">
-        <v>26.27</v>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>0-0</t>
-        </is>
-      </c>
-      <c r="T7" s="2" t="n">
-        <v>73.69999999999999</v>
-      </c>
-      <c r="U7" t="n">
-        <v>58.06</v>
+      <c r="T7" t="n">
+        <v>68.28999999999999</v>
+      </c>
+      <c r="U7" s="2" t="n">
+        <v>71.91</v>
       </c>
       <c r="V7" t="n">
-        <v>68.17999999999999</v>
-      </c>
-      <c r="W7" t="n">
-        <v>65.45</v>
-      </c>
-      <c r="X7" s="2" t="n">
-        <v>75.93000000000001</v>
-      </c>
-      <c r="Y7" t="n">
-        <v>69.70999999999999</v>
-      </c>
-      <c r="Z7" t="n">
-        <v>65.56999999999999</v>
+        <v>58.90000000000001</v>
+      </c>
+      <c r="W7" s="2" t="n">
+        <v>85.13</v>
+      </c>
+      <c r="X7" t="n">
+        <v>50.13</v>
+      </c>
+      <c r="Y7" s="2" t="n">
+        <v>88.56999999999999</v>
+      </c>
+      <c r="Z7" s="2" t="n">
+        <v>90.12</v>
       </c>
       <c r="AA7" t="n">
-        <v>33.53</v>
+        <v>63.92</v>
       </c>
       <c r="AB7" t="n">
-        <v>28.86</v>
-      </c>
-      <c r="AC7" s="2" t="n">
-        <v>88.06999999999999</v>
-      </c>
-      <c r="AD7" s="2" t="n">
-        <v>90.70999999999999</v>
+        <v>67.41</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>62.82</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>58.89</v>
       </c>
     </row>
     <row r="8">
@@ -1211,98 +1211,98 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>PSG</t>
+          <t>Bayern</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Brest</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>74.91</v>
+          <t>Leverkusen</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>42.37</v>
       </c>
       <c r="E8" t="n">
-        <v>14.12</v>
+        <v>23.54</v>
       </c>
       <c r="F8" t="n">
-        <v>10.94</v>
+        <v>34.08</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
           <t>1-0</t>
         </is>
       </c>
-      <c r="H8" s="2" t="n">
-        <v>89.03</v>
+      <c r="H8" t="n">
+        <v>65.91</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>85.84999999999999</v>
+        <v>76.44999999999999</v>
       </c>
       <c r="J8" t="n">
-        <v>25.06</v>
-      </c>
-      <c r="K8" t="n">
-        <v>69.56</v>
+        <v>57.62</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>72.72</v>
       </c>
       <c r="L8" t="n">
-        <v>46.41</v>
+        <v>49.09</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>75.06999999999999</v>
+        <v>72.78</v>
       </c>
       <c r="N8" s="2" t="n">
-        <v>88.68000000000001</v>
+        <v>87.20999999999999</v>
       </c>
       <c r="O8" t="n">
-        <v>32.99</v>
+        <v>52.19</v>
       </c>
       <c r="P8" t="n">
-        <v>53.31</v>
+        <v>6.49</v>
       </c>
       <c r="Q8" t="n">
-        <v>32</v>
+        <v>41.82</v>
       </c>
       <c r="R8" t="n">
-        <v>14.35</v>
+        <v>51.55</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>1-0</t>
-        </is>
-      </c>
-      <c r="T8" s="2" t="n">
-        <v>85.31</v>
+          <t>0-0</t>
+        </is>
+      </c>
+      <c r="T8" t="n">
+        <v>48.31</v>
       </c>
       <c r="U8" t="n">
-        <v>67.66</v>
-      </c>
-      <c r="V8" t="n">
-        <v>46.35</v>
-      </c>
-      <c r="W8" s="2" t="n">
-        <v>74.87</v>
-      </c>
-      <c r="X8" t="n">
-        <v>64.54000000000001</v>
+        <v>58.04</v>
+      </c>
+      <c r="V8" s="2" t="n">
+        <v>93.37</v>
+      </c>
+      <c r="W8" t="n">
+        <v>61.36</v>
+      </c>
+      <c r="X8" s="2" t="n">
+        <v>76.88</v>
       </c>
       <c r="Y8" s="2" t="n">
-        <v>86.54000000000001</v>
-      </c>
-      <c r="Z8" t="n">
-        <v>40.82</v>
+        <v>75.53</v>
+      </c>
+      <c r="Z8" s="2" t="n">
+        <v>70.76000000000001</v>
       </c>
       <c r="AA8" t="n">
-        <v>59.57</v>
+        <v>41.09</v>
       </c>
       <c r="AB8" t="n">
-        <v>9.779999999999999</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>67.47</v>
+        <v>34.8</v>
+      </c>
+      <c r="AC8" s="2" t="n">
+        <v>83.16</v>
       </c>
       <c r="AD8" s="2" t="n">
-        <v>98.34</v>
+        <v>87.3</v>
       </c>
     </row>
     <row r="9">
@@ -1313,60 +1313,60 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>PSG</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Man City</t>
-        </is>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>77.8</v>
+          <t>Liverpool</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>29.67</v>
       </c>
       <c r="E9" t="n">
-        <v>9.49</v>
+        <v>25.44</v>
       </c>
       <c r="F9" t="n">
-        <v>11.07</v>
+        <v>44.89</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>3-1</t>
-        </is>
-      </c>
-      <c r="H9" s="2" t="n">
-        <v>87.28999999999999</v>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>55.11</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>88.87</v>
-      </c>
-      <c r="J9" t="n">
-        <v>20.56</v>
-      </c>
-      <c r="K9" s="2" t="n">
-        <v>94.48</v>
-      </c>
-      <c r="L9" s="2" t="n">
-        <v>88.33</v>
-      </c>
-      <c r="M9" t="n">
-        <v>22.33</v>
-      </c>
-      <c r="N9" t="n">
-        <v>38.67</v>
-      </c>
-      <c r="O9" s="2" t="n">
-        <v>73.95999999999999</v>
+        <v>74.56</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>70.33</v>
+      </c>
+      <c r="K9" t="n">
+        <v>65.13</v>
+      </c>
+      <c r="L9" t="n">
+        <v>39.86</v>
+      </c>
+      <c r="M9" s="2" t="n">
+        <v>80.34</v>
+      </c>
+      <c r="N9" s="2" t="n">
+        <v>91.86</v>
+      </c>
+      <c r="O9" t="n">
+        <v>44.18</v>
       </c>
       <c r="P9" t="n">
-        <v>19.23</v>
+        <v>30.79</v>
       </c>
       <c r="Q9" t="n">
-        <v>42.87</v>
+        <v>37.18</v>
       </c>
       <c r="R9" t="n">
-        <v>37.86</v>
+        <v>31.94</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
@@ -1374,37 +1374,37 @@
         </is>
       </c>
       <c r="T9" t="n">
-        <v>62.09999999999999</v>
+        <v>67.97</v>
       </c>
       <c r="U9" t="n">
-        <v>57.09</v>
-      </c>
-      <c r="V9" s="2" t="n">
-        <v>80.72999999999999</v>
-      </c>
-      <c r="W9" t="n">
-        <v>63.53</v>
-      </c>
-      <c r="X9" s="2" t="n">
-        <v>77.26000000000001</v>
-      </c>
-      <c r="Y9" s="2" t="n">
-        <v>96.16</v>
+        <v>62.73</v>
+      </c>
+      <c r="V9" t="n">
+        <v>69.12</v>
+      </c>
+      <c r="W9" s="2" t="n">
+        <v>72.44</v>
+      </c>
+      <c r="X9" t="n">
+        <v>68.08</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>62.69</v>
       </c>
       <c r="Z9" s="2" t="n">
-        <v>76.45999999999999</v>
-      </c>
-      <c r="AA9" s="2" t="n">
-        <v>87.75</v>
+        <v>72.59</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>25.9</v>
       </c>
       <c r="AB9" t="n">
-        <v>43.56</v>
-      </c>
-      <c r="AC9" t="n">
-        <v>26.64</v>
+        <v>37.11</v>
+      </c>
+      <c r="AC9" s="2" t="n">
+        <v>92.23</v>
       </c>
       <c r="AD9" s="2" t="n">
-        <v>79.51000000000001</v>
+        <v>85.84</v>
       </c>
     </row>
     <row r="10">
@@ -1415,22 +1415,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Bodo Glimt</t>
+          <t>AZ Alkmaar</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Twente</t>
+          <t>Tottenham</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>42.98</v>
+        <v>35.69</v>
       </c>
       <c r="E10" t="n">
-        <v>26.4</v>
+        <v>23.92</v>
       </c>
       <c r="F10" t="n">
-        <v>30.62</v>
+        <v>40.38</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1438,37 +1438,37 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>69.38</v>
+        <v>59.61</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>73.59999999999999</v>
+        <v>76.06999999999999</v>
       </c>
       <c r="J10" t="n">
-        <v>57.02</v>
+        <v>64.30000000000001</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>70.95</v>
+        <v>79.41</v>
       </c>
       <c r="L10" t="n">
-        <v>45.44</v>
-      </c>
-      <c r="M10" s="2" t="n">
-        <v>75.90000000000001</v>
+        <v>57.03</v>
+      </c>
+      <c r="M10" t="n">
+        <v>65.37</v>
       </c>
       <c r="N10" s="2" t="n">
-        <v>89.20999999999999</v>
+        <v>82.01000000000001</v>
       </c>
       <c r="O10" t="n">
-        <v>50.1</v>
+        <v>59.55</v>
       </c>
       <c r="P10" t="n">
-        <v>27.28</v>
+        <v>21.46</v>
       </c>
       <c r="Q10" t="n">
-        <v>50.55</v>
+        <v>52.32</v>
       </c>
       <c r="R10" t="n">
-        <v>22.1</v>
+        <v>26.2</v>
       </c>
       <c r="S10" t="inlineStr">
         <is>
@@ -1476,37 +1476,37 @@
         </is>
       </c>
       <c r="T10" s="2" t="n">
-        <v>77.83</v>
+        <v>73.78</v>
       </c>
       <c r="U10" t="n">
-        <v>49.38</v>
+        <v>47.66</v>
       </c>
       <c r="V10" s="2" t="n">
-        <v>72.65000000000001</v>
+        <v>78.52</v>
       </c>
       <c r="W10" t="n">
-        <v>64.66</v>
-      </c>
-      <c r="X10" t="n">
-        <v>63.87</v>
+        <v>56.86</v>
+      </c>
+      <c r="X10" s="2" t="n">
+        <v>77.54000000000001</v>
       </c>
       <c r="Y10" s="2" t="n">
-        <v>74.75</v>
-      </c>
-      <c r="Z10" t="n">
-        <v>67.26000000000001</v>
+        <v>76.12</v>
+      </c>
+      <c r="Z10" s="2" t="n">
+        <v>78.53</v>
       </c>
       <c r="AA10" t="n">
-        <v>40</v>
+        <v>41.93</v>
       </c>
       <c r="AB10" t="n">
-        <v>30.71</v>
+        <v>45.51</v>
       </c>
       <c r="AC10" s="2" t="n">
-        <v>83.91</v>
+        <v>82.56</v>
       </c>
       <c r="AD10" s="2" t="n">
-        <v>89.7</v>
+        <v>79.90000000000001</v>
       </c>
     </row>
     <row r="11">
@@ -1522,93 +1522,93 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>PAOK</t>
+          <t>Lyon</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>51.26</v>
+        <v>37.38</v>
       </c>
       <c r="E11" t="n">
-        <v>25.39</v>
+        <v>26.65</v>
       </c>
       <c r="F11" t="n">
-        <v>23.35</v>
+        <v>35.97</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>1-0</t>
-        </is>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>76.65000000000001</v>
+          <t>1-1</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>64.03</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>74.61</v>
+        <v>73.34999999999999</v>
       </c>
       <c r="J11" t="n">
-        <v>48.74</v>
+        <v>62.62</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>70.51000000000001</v>
+        <v>70.38</v>
       </c>
       <c r="L11" t="n">
-        <v>44.89</v>
+        <v>44.84</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>76.36</v>
+        <v>76.40000000000001</v>
       </c>
       <c r="N11" s="2" t="n">
-        <v>89.48999999999999</v>
+        <v>89.52</v>
       </c>
       <c r="O11" t="n">
-        <v>47.59</v>
+        <v>50.01</v>
       </c>
       <c r="P11" t="n">
-        <v>23.49</v>
+        <v>19.6</v>
       </c>
       <c r="Q11" t="n">
-        <v>54.63</v>
+        <v>48.02</v>
       </c>
       <c r="R11" t="n">
-        <v>21.85</v>
+        <v>32.33</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
           <t>0-0</t>
         </is>
       </c>
-      <c r="T11" s="2" t="n">
-        <v>78.12</v>
+      <c r="T11" t="n">
+        <v>67.62</v>
       </c>
       <c r="U11" t="n">
-        <v>45.34</v>
+        <v>51.93</v>
       </c>
       <c r="V11" s="2" t="n">
-        <v>76.48</v>
+        <v>80.34999999999999</v>
       </c>
       <c r="W11" t="n">
-        <v>57.6</v>
+        <v>62.72</v>
       </c>
       <c r="X11" s="2" t="n">
-        <v>72.72</v>
+        <v>71.69</v>
       </c>
       <c r="Y11" s="2" t="n">
-        <v>78.38</v>
-      </c>
-      <c r="Z11" t="n">
-        <v>60.94</v>
+        <v>71.34</v>
+      </c>
+      <c r="Z11" s="2" t="n">
+        <v>70.48</v>
       </c>
       <c r="AA11" t="n">
-        <v>45.27</v>
+        <v>35.52</v>
       </c>
       <c r="AB11" t="n">
-        <v>24.22</v>
+        <v>34.47</v>
       </c>
       <c r="AC11" s="2" t="n">
-        <v>80.08</v>
+        <v>86.84999999999999</v>
       </c>
       <c r="AD11" s="2" t="n">
-        <v>93.03</v>
+        <v>87.51000000000001</v>
       </c>
     </row>
     <row r="12">
@@ -1619,98 +1619,98 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Galatasaray</t>
+          <t>Fenerbahce</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>AZ Alkmaar</t>
+          <t>Rangers</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>43.03</v>
+        <v>34.01</v>
       </c>
       <c r="E12" t="n">
-        <v>18.35</v>
+        <v>22.69</v>
       </c>
       <c r="F12" t="n">
-        <v>38.42</v>
+        <v>43.3</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2-2</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>61.38</v>
+        <v>56.7</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>81.45</v>
+        <v>77.31</v>
       </c>
       <c r="J12" t="n">
-        <v>56.77</v>
+        <v>65.98999999999999</v>
       </c>
       <c r="K12" s="2" t="n">
-        <v>95.41</v>
-      </c>
-      <c r="L12" s="2" t="n">
-        <v>86.66</v>
+        <v>83.18000000000001</v>
+      </c>
+      <c r="L12" t="n">
+        <v>62.85</v>
       </c>
       <c r="M12" t="n">
-        <v>27.61</v>
-      </c>
-      <c r="N12" t="n">
-        <v>45.43</v>
-      </c>
-      <c r="O12" s="2" t="n">
-        <v>83.37</v>
+        <v>59.34</v>
+      </c>
+      <c r="N12" s="2" t="n">
+        <v>77.33</v>
+      </c>
+      <c r="O12" t="n">
+        <v>63.89</v>
       </c>
       <c r="P12" t="n">
-        <v>45.18</v>
+        <v>10.97</v>
       </c>
       <c r="Q12" t="n">
-        <v>32.17</v>
+        <v>29.94</v>
       </c>
       <c r="R12" t="n">
-        <v>19.05</v>
+        <v>57.66</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>1-1</t>
-        </is>
-      </c>
-      <c r="T12" s="2" t="n">
-        <v>77.34999999999999</v>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="T12" t="n">
+        <v>40.91</v>
       </c>
       <c r="U12" t="n">
-        <v>64.23</v>
-      </c>
-      <c r="V12" t="n">
-        <v>51.22</v>
+        <v>68.63</v>
+      </c>
+      <c r="V12" s="2" t="n">
+        <v>87.59999999999999</v>
       </c>
       <c r="W12" s="2" t="n">
-        <v>86.15000000000001</v>
+        <v>81.79000000000001</v>
       </c>
       <c r="X12" t="n">
-        <v>18.92</v>
+        <v>43.06</v>
       </c>
       <c r="Y12" s="2" t="n">
-        <v>91.81</v>
+        <v>77.92</v>
       </c>
       <c r="Z12" s="2" t="n">
-        <v>90.68000000000001</v>
-      </c>
-      <c r="AA12" s="2" t="n">
-        <v>71.65000000000001</v>
+        <v>82.26000000000001</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>44.58</v>
       </c>
       <c r="AB12" t="n">
-        <v>68.87</v>
-      </c>
-      <c r="AC12" t="n">
-        <v>53.63</v>
-      </c>
-      <c r="AD12" t="n">
-        <v>57.04</v>
+        <v>51.6</v>
+      </c>
+      <c r="AC12" s="2" t="n">
+        <v>80.59999999999999</v>
+      </c>
+      <c r="AD12" s="2" t="n">
+        <v>74.92</v>
       </c>
     </row>
     <row r="13">
@@ -1721,98 +1721,98 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Roma</t>
+          <t>Real Sociedad</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Porto</t>
+          <t>Man Utd</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>50.5</v>
+        <v>34.98</v>
       </c>
       <c r="E13" t="n">
-        <v>28.27</v>
+        <v>23.39</v>
       </c>
       <c r="F13" t="n">
-        <v>21.23</v>
+        <v>41.63</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>1-0</t>
-        </is>
-      </c>
-      <c r="H13" s="2" t="n">
-        <v>78.77</v>
+          <t>1-1</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>58.37</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>71.73</v>
+        <v>76.61</v>
       </c>
       <c r="J13" t="n">
-        <v>49.5</v>
-      </c>
-      <c r="K13" t="n">
-        <v>60.78</v>
+        <v>65.02000000000001</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>81.08</v>
       </c>
       <c r="L13" t="n">
-        <v>33.92</v>
-      </c>
-      <c r="M13" s="2" t="n">
-        <v>84.64</v>
+        <v>59.54</v>
+      </c>
+      <c r="M13" t="n">
+        <v>62.83</v>
       </c>
       <c r="N13" s="2" t="n">
-        <v>94.19</v>
+        <v>80.09</v>
       </c>
       <c r="O13" t="n">
-        <v>38.16</v>
+        <v>61.44</v>
       </c>
       <c r="P13" t="n">
-        <v>43.23</v>
+        <v>28.18</v>
       </c>
       <c r="Q13" t="n">
-        <v>47.14</v>
+        <v>33.33</v>
       </c>
       <c r="R13" t="n">
-        <v>9.470000000000001</v>
+        <v>37.57</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>0-0</t>
-        </is>
-      </c>
-      <c r="T13" s="2" t="n">
-        <v>90.37</v>
+          <t>1-1</t>
+        </is>
+      </c>
+      <c r="T13" t="n">
+        <v>61.51</v>
       </c>
       <c r="U13" t="n">
-        <v>52.7</v>
-      </c>
-      <c r="V13" t="n">
-        <v>56.61</v>
-      </c>
-      <c r="W13" t="n">
-        <v>63.88</v>
+        <v>65.75</v>
+      </c>
+      <c r="V13" s="2" t="n">
+        <v>70.90000000000001</v>
+      </c>
+      <c r="W13" s="2" t="n">
+        <v>84.94</v>
       </c>
       <c r="X13" t="n">
-        <v>66.77</v>
+        <v>36.63</v>
       </c>
       <c r="Y13" s="2" t="n">
-        <v>73.2</v>
-      </c>
-      <c r="Z13" t="n">
-        <v>52.38</v>
+        <v>76.90000000000001</v>
+      </c>
+      <c r="Z13" s="2" t="n">
+        <v>80.18000000000001</v>
       </c>
       <c r="AA13" t="n">
-        <v>37.91</v>
+        <v>43.06</v>
       </c>
       <c r="AB13" t="n">
-        <v>17.05</v>
+        <v>48.11</v>
       </c>
       <c r="AC13" s="2" t="n">
-        <v>85.31999999999999</v>
+        <v>81.73999999999999</v>
       </c>
       <c r="AD13" s="2" t="n">
-        <v>96.05</v>
+        <v>77.84999999999999</v>
       </c>
     </row>
     <row r="14">
@@ -1828,55 +1828,55 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>USG</t>
+          <t>Frankfurt</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>63.16</v>
+        <v>51.03</v>
       </c>
       <c r="E14" t="n">
-        <v>23.92</v>
+        <v>23.04</v>
       </c>
       <c r="F14" t="n">
-        <v>12.92</v>
+        <v>25.92</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>87.08</v>
+        <v>74.06999999999999</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>76.08</v>
+        <v>76.95</v>
       </c>
       <c r="J14" t="n">
-        <v>36.84</v>
-      </c>
-      <c r="K14" t="n">
-        <v>64.04000000000001</v>
+        <v>48.96</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>78.89</v>
       </c>
       <c r="L14" t="n">
-        <v>37.34</v>
-      </c>
-      <c r="M14" s="2" t="n">
-        <v>82.22</v>
+        <v>56.26</v>
+      </c>
+      <c r="M14" t="n">
+        <v>66.12</v>
       </c>
       <c r="N14" s="2" t="n">
-        <v>92.91</v>
+        <v>82.56999999999999</v>
       </c>
       <c r="O14" t="n">
-        <v>34.62</v>
+        <v>57.12</v>
       </c>
       <c r="P14" t="n">
-        <v>42.02</v>
+        <v>24.95</v>
       </c>
       <c r="Q14" t="n">
-        <v>56.72</v>
+        <v>61.71</v>
       </c>
       <c r="R14" t="n">
-        <v>1.23</v>
+        <v>13.34</v>
       </c>
       <c r="S14" t="inlineStr">
         <is>
@@ -1884,37 +1884,37 @@
         </is>
       </c>
       <c r="T14" s="2" t="n">
-        <v>98.74000000000001</v>
+        <v>86.66</v>
       </c>
       <c r="U14" t="n">
-        <v>43.25</v>
-      </c>
-      <c r="V14" t="n">
-        <v>57.95</v>
+        <v>38.29</v>
+      </c>
+      <c r="V14" s="2" t="n">
+        <v>75.05</v>
       </c>
       <c r="W14" t="n">
-        <v>44.43</v>
+        <v>43.29</v>
       </c>
       <c r="X14" s="2" t="n">
-        <v>87.69</v>
+        <v>87.98999999999999</v>
       </c>
       <c r="Y14" s="2" t="n">
-        <v>80.14</v>
+        <v>82.7</v>
       </c>
       <c r="Z14" t="n">
-        <v>43.38</v>
+        <v>69.33</v>
       </c>
       <c r="AA14" t="n">
-        <v>48.04</v>
+        <v>52.36</v>
       </c>
       <c r="AB14" t="n">
-        <v>11.18</v>
+        <v>33.09</v>
       </c>
       <c r="AC14" s="2" t="n">
-        <v>77.90000000000001</v>
+        <v>74.26000000000001</v>
       </c>
       <c r="AD14" s="2" t="n">
-        <v>97.98</v>
+        <v>88.31999999999999</v>
       </c>
     </row>
     <row r="15">
@@ -1925,60 +1925,60 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Anderlecht</t>
+          <t>Bodo Glimt</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Fenerbahce</t>
+          <t>Olympiacos</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>36.05</v>
+        <v>16.02</v>
       </c>
       <c r="E15" t="n">
-        <v>23.23</v>
+        <v>35.34</v>
       </c>
       <c r="F15" t="n">
-        <v>40.71</v>
+        <v>48.64</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>59.28</v>
-      </c>
-      <c r="I15" s="2" t="n">
-        <v>76.75999999999999</v>
-      </c>
-      <c r="J15" t="n">
-        <v>63.94</v>
-      </c>
-      <c r="K15" s="2" t="n">
-        <v>82.27</v>
+        <v>51.36</v>
+      </c>
+      <c r="I15" t="n">
+        <v>64.66</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>83.98</v>
+      </c>
+      <c r="K15" t="n">
+        <v>41.04</v>
       </c>
       <c r="L15" t="n">
-        <v>61.29</v>
-      </c>
-      <c r="M15" t="n">
-        <v>61.01</v>
+        <v>16.96</v>
+      </c>
+      <c r="M15" s="2" t="n">
+        <v>94.48</v>
       </c>
       <c r="N15" s="2" t="n">
-        <v>78.66</v>
+        <v>98.52</v>
       </c>
       <c r="O15" t="n">
-        <v>62.93</v>
+        <v>21.64</v>
       </c>
       <c r="P15" t="n">
-        <v>25.66</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>45.91</v>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="2" t="n">
+        <v>70.58</v>
       </c>
       <c r="R15" t="n">
-        <v>28.21</v>
+        <v>29.41</v>
       </c>
       <c r="S15" t="inlineStr">
         <is>
@@ -1986,37 +1986,37 @@
         </is>
       </c>
       <c r="T15" s="2" t="n">
-        <v>71.56999999999999</v>
+        <v>70.58</v>
       </c>
       <c r="U15" t="n">
-        <v>53.87</v>
+        <v>29.41</v>
       </c>
       <c r="V15" s="2" t="n">
-        <v>74.12</v>
-      </c>
-      <c r="W15" s="2" t="n">
-        <v>73.02</v>
-      </c>
-      <c r="X15" t="n">
-        <v>50.81</v>
-      </c>
-      <c r="Y15" s="2" t="n">
-        <v>78.31</v>
-      </c>
-      <c r="Z15" s="2" t="n">
-        <v>80.54000000000001</v>
+        <v>99.98999999999999</v>
+      </c>
+      <c r="W15" t="n">
+        <v>29.41</v>
+      </c>
+      <c r="X15" s="2" t="n">
+        <v>95.17</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>34.92</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>62.59</v>
       </c>
       <c r="AA15" t="n">
-        <v>45.17</v>
+        <v>6.96</v>
       </c>
       <c r="AB15" t="n">
-        <v>48.7</v>
+        <v>25.81</v>
       </c>
       <c r="AC15" s="2" t="n">
-        <v>80.16</v>
+        <v>99.04000000000001</v>
       </c>
       <c r="AD15" s="2" t="n">
-        <v>77.36</v>
+        <v>92.28</v>
       </c>
     </row>
     <row r="16">
@@ -2027,22 +2027,22 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Real Sociedad</t>
+          <t>Roma</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Midtjylland</t>
+          <t>Athletic Bilbao</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>61.88</v>
+        <v>42.68</v>
       </c>
       <c r="E16" t="n">
-        <v>22.31</v>
+        <v>27.67</v>
       </c>
       <c r="F16" t="n">
-        <v>15.8</v>
+        <v>29.66</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -2050,37 +2050,37 @@
         </is>
       </c>
       <c r="H16" s="2" t="n">
-        <v>84.19</v>
+        <v>70.34999999999999</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>77.68000000000001</v>
+        <v>72.34</v>
       </c>
       <c r="J16" t="n">
-        <v>38.11</v>
-      </c>
-      <c r="K16" s="2" t="n">
-        <v>72.47</v>
+        <v>57.33</v>
+      </c>
+      <c r="K16" t="n">
+        <v>66.12</v>
       </c>
       <c r="L16" t="n">
-        <v>47.34</v>
+        <v>39.8</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>74.3</v>
+        <v>80.39</v>
       </c>
       <c r="N16" s="2" t="n">
-        <v>88.19</v>
+        <v>91.89</v>
       </c>
       <c r="O16" t="n">
-        <v>44.72</v>
+        <v>45.38</v>
       </c>
       <c r="P16" t="n">
-        <v>53.66</v>
+        <v>35.8</v>
       </c>
       <c r="Q16" t="n">
-        <v>33.36</v>
+        <v>42.72</v>
       </c>
       <c r="R16" t="n">
-        <v>10.78</v>
+        <v>21.34</v>
       </c>
       <c r="S16" t="inlineStr">
         <is>
@@ -2088,37 +2088,37 @@
         </is>
       </c>
       <c r="T16" s="2" t="n">
-        <v>87.02</v>
+        <v>78.52</v>
       </c>
       <c r="U16" t="n">
-        <v>64.44</v>
+        <v>57.14</v>
       </c>
       <c r="V16" t="n">
-        <v>44.14</v>
+        <v>64.06</v>
       </c>
       <c r="W16" s="2" t="n">
-        <v>82.55</v>
+        <v>70.72</v>
       </c>
       <c r="X16" t="n">
-        <v>31.56</v>
+        <v>61.89</v>
       </c>
       <c r="Y16" s="2" t="n">
-        <v>83.38</v>
+        <v>71.93000000000001</v>
       </c>
       <c r="Z16" t="n">
-        <v>53.81</v>
+        <v>63.47</v>
       </c>
       <c r="AA16" t="n">
-        <v>53.57</v>
+        <v>36.26</v>
       </c>
       <c r="AB16" t="n">
-        <v>18.13</v>
+        <v>26.69</v>
       </c>
       <c r="AC16" s="2" t="n">
-        <v>73.18000000000001</v>
+        <v>86.39</v>
       </c>
       <c r="AD16" s="2" t="n">
-        <v>95.63</v>
+        <v>91.84</v>
       </c>
     </row>
     <row r="17">
@@ -2134,93 +2134,93 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Ferencvaros</t>
+          <t>Lazio</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>57.36</v>
+        <v>24.02</v>
       </c>
       <c r="E17" t="n">
-        <v>20.8</v>
+        <v>26.04</v>
       </c>
       <c r="F17" t="n">
-        <v>21.81</v>
+        <v>49.94</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2-1</t>
-        </is>
-      </c>
-      <c r="H17" s="2" t="n">
-        <v>78.16</v>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>50.06</v>
       </c>
       <c r="I17" s="2" t="n">
-        <v>79.17</v>
-      </c>
-      <c r="J17" t="n">
-        <v>42.61</v>
-      </c>
-      <c r="K17" s="2" t="n">
-        <v>83.45</v>
+        <v>73.95999999999999</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>75.97999999999999</v>
+      </c>
+      <c r="K17" t="n">
+        <v>68.40000000000001</v>
       </c>
       <c r="L17" t="n">
-        <v>63.17</v>
-      </c>
-      <c r="M17" t="n">
-        <v>58.97</v>
+        <v>42.44</v>
+      </c>
+      <c r="M17" s="2" t="n">
+        <v>78.34</v>
       </c>
       <c r="N17" s="2" t="n">
-        <v>77.03</v>
+        <v>90.69</v>
       </c>
       <c r="O17" t="n">
-        <v>60.75</v>
+        <v>45.87</v>
       </c>
       <c r="P17" t="n">
-        <v>28.59</v>
+        <v>18.02</v>
       </c>
       <c r="Q17" t="n">
-        <v>50.64</v>
+        <v>43.16</v>
       </c>
       <c r="R17" t="n">
-        <v>20.7</v>
+        <v>38.69</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
           <t>0-0</t>
         </is>
       </c>
-      <c r="T17" s="2" t="n">
-        <v>79.23</v>
+      <c r="T17" t="n">
+        <v>61.17999999999999</v>
       </c>
       <c r="U17" t="n">
-        <v>49.29</v>
+        <v>56.70999999999999</v>
       </c>
       <c r="V17" s="2" t="n">
-        <v>71.34</v>
+        <v>81.84999999999999</v>
       </c>
       <c r="W17" t="n">
-        <v>64.28</v>
+        <v>69.13</v>
       </c>
       <c r="X17" t="n">
-        <v>64.45999999999999</v>
-      </c>
-      <c r="Y17" s="2" t="n">
-        <v>87.23</v>
-      </c>
-      <c r="Z17" t="n">
-        <v>69.78</v>
+        <v>64.12</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>60.12</v>
+      </c>
+      <c r="Z17" s="2" t="n">
+        <v>76.73</v>
       </c>
       <c r="AA17" t="n">
-        <v>60.97</v>
+        <v>23.45</v>
       </c>
       <c r="AB17" t="n">
-        <v>33.64</v>
-      </c>
-      <c r="AC17" t="n">
-        <v>66.04000000000001</v>
+        <v>42.81</v>
+      </c>
+      <c r="AC17" s="2" t="n">
+        <v>93.39</v>
       </c>
       <c r="AD17" s="2" t="n">
-        <v>87.98</v>
+        <v>81.92</v>
       </c>
     </row>
     <row r="18">
@@ -2231,98 +2231,98 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Heidenheim</t>
+          <t>Copenhagen</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Copenhagen</t>
+          <t>Chelsea</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>68.77</v>
+        <v>1.82</v>
       </c>
       <c r="E18" t="n">
-        <v>20.43</v>
-      </c>
-      <c r="F18" t="n">
-        <v>10.77</v>
+        <v>2.91</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>80.48</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2-0</t>
-        </is>
-      </c>
-      <c r="H18" s="2" t="n">
-        <v>89.19999999999999</v>
+          <t>1-5</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>4.73</v>
       </c>
       <c r="I18" s="2" t="n">
-        <v>79.53999999999999</v>
-      </c>
-      <c r="J18" t="n">
-        <v>31.2</v>
+        <v>82.3</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>83.39</v>
       </c>
       <c r="K18" s="2" t="n">
-        <v>75.59</v>
-      </c>
-      <c r="L18" t="n">
-        <v>50.62</v>
-      </c>
-      <c r="M18" s="2" t="n">
-        <v>71.40000000000001</v>
-      </c>
-      <c r="N18" s="2" t="n">
-        <v>86.28</v>
+        <v>84.54000000000001</v>
+      </c>
+      <c r="L18" s="2" t="n">
+        <v>82.62</v>
+      </c>
+      <c r="M18" t="n">
+        <v>7.28</v>
+      </c>
+      <c r="N18" t="n">
+        <v>15.72</v>
       </c>
       <c r="O18" t="n">
-        <v>42.91</v>
+        <v>60.02</v>
       </c>
       <c r="P18" t="n">
-        <v>34.16</v>
+        <v>5.34</v>
       </c>
       <c r="Q18" t="n">
-        <v>57.99</v>
+        <v>11.79</v>
       </c>
       <c r="R18" t="n">
-        <v>7.84</v>
+        <v>68.16</v>
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>0-0</t>
-        </is>
-      </c>
-      <c r="T18" s="2" t="n">
-        <v>92.15000000000001</v>
-      </c>
-      <c r="U18" t="n">
-        <v>42</v>
-      </c>
-      <c r="V18" t="n">
-        <v>65.83</v>
-      </c>
-      <c r="W18" t="n">
-        <v>46.77</v>
-      </c>
-      <c r="X18" s="2" t="n">
-        <v>85.42</v>
-      </c>
-      <c r="Y18" s="2" t="n">
-        <v>86.83</v>
-      </c>
-      <c r="Z18" t="n">
-        <v>48.87</v>
+          <t>0-2</t>
+        </is>
+      </c>
+      <c r="T18" t="n">
+        <v>17.13</v>
+      </c>
+      <c r="U18" s="2" t="n">
+        <v>73.5</v>
+      </c>
+      <c r="V18" s="2" t="n">
+        <v>79.94999999999999</v>
+      </c>
+      <c r="W18" s="2" t="n">
+        <v>81.78</v>
+      </c>
+      <c r="X18" t="n">
+        <v>15.4</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>60.24</v>
+      </c>
+      <c r="Z18" s="2" t="n">
+        <v>84.95</v>
       </c>
       <c r="AA18" t="n">
-        <v>60.16</v>
-      </c>
-      <c r="AB18" t="n">
-        <v>14.58</v>
-      </c>
-      <c r="AC18" t="n">
-        <v>66.87</v>
-      </c>
-      <c r="AD18" s="2" t="n">
-        <v>96.90000000000001</v>
+        <v>29.6</v>
+      </c>
+      <c r="AB18" s="2" t="n">
+        <v>83.40000000000001</v>
+      </c>
+      <c r="AC18" s="2" t="n">
+        <v>74.42</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>6.41</v>
       </c>
     </row>
     <row r="19">
@@ -2333,98 +2333,98 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Olimpija</t>
+          <t>Molde</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Borac</t>
+          <t>Legia</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>36.51</v>
+        <v>18.35</v>
       </c>
       <c r="E19" t="n">
-        <v>38.98</v>
+        <v>20.11</v>
       </c>
       <c r="F19" t="n">
-        <v>24.51</v>
+        <v>61.52</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>0-0</t>
-        </is>
-      </c>
-      <c r="H19" s="2" t="n">
-        <v>75.48999999999999</v>
-      </c>
-      <c r="I19" t="n">
-        <v>61.02</v>
-      </c>
-      <c r="J19" t="n">
-        <v>63.48999999999999</v>
-      </c>
-      <c r="K19" t="n">
-        <v>41.94</v>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>38.46</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>79.87</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>81.63</v>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>77.56999999999999</v>
       </c>
       <c r="L19" t="n">
-        <v>17.01</v>
-      </c>
-      <c r="M19" s="2" t="n">
-        <v>94.45999999999999</v>
+        <v>55.03</v>
+      </c>
+      <c r="M19" t="n">
+        <v>67.3</v>
       </c>
       <c r="N19" s="2" t="n">
-        <v>98.52</v>
+        <v>83.42</v>
       </c>
       <c r="O19" t="n">
-        <v>25.83</v>
+        <v>51.51</v>
       </c>
       <c r="P19" t="n">
-        <v>25.13</v>
-      </c>
-      <c r="Q19" s="2" t="n">
-        <v>74.87</v>
+        <v>42.23</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>32.66</v>
       </c>
       <c r="R19" t="n">
-        <v>0</v>
+        <v>24.61</v>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>0-0</t>
+          <t>1-0</t>
         </is>
       </c>
       <c r="T19" s="2" t="n">
-        <v>100</v>
+        <v>74.88999999999999</v>
       </c>
       <c r="U19" t="n">
-        <v>25.13</v>
-      </c>
-      <c r="V19" s="2" t="n">
-        <v>74.87</v>
-      </c>
-      <c r="W19" t="n">
-        <v>25.13</v>
-      </c>
-      <c r="X19" s="2" t="n">
-        <v>96.54000000000001</v>
+        <v>66.84</v>
+      </c>
+      <c r="V19" t="n">
+        <v>57.27</v>
+      </c>
+      <c r="W19" s="2" t="n">
+        <v>82.14</v>
+      </c>
+      <c r="X19" t="n">
+        <v>48</v>
       </c>
       <c r="Y19" t="n">
-        <v>55.41</v>
-      </c>
-      <c r="Z19" t="n">
-        <v>45.5</v>
+        <v>60.93</v>
+      </c>
+      <c r="Z19" s="2" t="n">
+        <v>85.68000000000001</v>
       </c>
       <c r="AA19" t="n">
-        <v>19.4</v>
+        <v>24.22</v>
       </c>
       <c r="AB19" t="n">
-        <v>12.42</v>
+        <v>57.86</v>
       </c>
       <c r="AC19" s="2" t="n">
-        <v>95.15000000000001</v>
-      </c>
-      <c r="AD19" s="2" t="n">
-        <v>97.62</v>
+        <v>93.02</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>69.17</v>
       </c>
     </row>
     <row r="20">
@@ -2435,60 +2435,60 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Pafos</t>
+          <t>Panathinaikos</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Omonia</t>
+          <t>Fiorentina</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>69.8</v>
+        <v>32.57</v>
       </c>
       <c r="E20" t="n">
-        <v>19.73</v>
+        <v>21.13</v>
       </c>
       <c r="F20" t="n">
-        <v>10.44</v>
+        <v>46.29</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2-0</t>
-        </is>
-      </c>
-      <c r="H20" s="2" t="n">
-        <v>89.53</v>
+          <t>1-1</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>53.7</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>80.23999999999999</v>
+        <v>78.86</v>
       </c>
       <c r="J20" t="n">
-        <v>30.17</v>
+        <v>67.42</v>
       </c>
       <c r="K20" s="2" t="n">
-        <v>76.97</v>
+        <v>84.2</v>
       </c>
       <c r="L20" t="n">
-        <v>52.55</v>
+        <v>65.29000000000001</v>
       </c>
       <c r="M20" t="n">
-        <v>69.64</v>
+        <v>56.65</v>
       </c>
       <c r="N20" s="2" t="n">
-        <v>85.08</v>
+        <v>75.09999999999999</v>
       </c>
       <c r="O20" t="n">
-        <v>43.83</v>
+        <v>65.05</v>
       </c>
       <c r="P20" t="n">
-        <v>54.38</v>
+        <v>56.54</v>
       </c>
       <c r="Q20" t="n">
-        <v>45.48</v>
+        <v>39.14</v>
       </c>
       <c r="R20" t="n">
-        <v>0</v>
+        <v>4.05</v>
       </c>
       <c r="S20" t="inlineStr">
         <is>
@@ -2496,37 +2496,37 @@
         </is>
       </c>
       <c r="T20" s="2" t="n">
-        <v>99.86</v>
+        <v>95.68000000000001</v>
       </c>
       <c r="U20" t="n">
-        <v>54.38</v>
+        <v>60.59</v>
       </c>
       <c r="V20" t="n">
-        <v>45.48</v>
+        <v>43.19</v>
       </c>
       <c r="W20" t="n">
-        <v>54.38</v>
+        <v>64.04000000000001</v>
       </c>
       <c r="X20" s="2" t="n">
-        <v>81.31999999999999</v>
+        <v>72.52</v>
       </c>
       <c r="Y20" s="2" t="n">
-        <v>87.69</v>
-      </c>
-      <c r="Z20" t="n">
-        <v>49.44</v>
+        <v>78.04000000000001</v>
+      </c>
+      <c r="Z20" s="2" t="n">
+        <v>84.2</v>
       </c>
       <c r="AA20" t="n">
-        <v>61.95</v>
+        <v>44.76</v>
       </c>
       <c r="AB20" t="n">
-        <v>14.97</v>
-      </c>
-      <c r="AC20" t="n">
-        <v>65.02</v>
+        <v>55.07</v>
+      </c>
+      <c r="AC20" s="2" t="n">
+        <v>80.45999999999999</v>
       </c>
       <c r="AD20" s="2" t="n">
-        <v>96.76000000000001</v>
+        <v>71.81</v>
       </c>
     </row>
     <row r="21">
@@ -2542,55 +2542,55 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Gent</t>
+          <t>Vitoria</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>54.01</v>
+        <v>26.47</v>
       </c>
       <c r="E21" t="n">
-        <v>34.61</v>
+        <v>35.43</v>
       </c>
       <c r="F21" t="n">
-        <v>11.37</v>
+        <v>38.1</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>1-0</t>
-        </is>
-      </c>
-      <c r="H21" s="2" t="n">
-        <v>88.62</v>
+          <t>0-0</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>61.9</v>
       </c>
       <c r="I21" t="n">
-        <v>65.38</v>
-      </c>
-      <c r="J21" t="n">
-        <v>45.98</v>
+        <v>64.56999999999999</v>
+      </c>
+      <c r="J21" s="2" t="n">
+        <v>73.53</v>
       </c>
       <c r="K21" t="n">
-        <v>42.57</v>
+        <v>41.91</v>
       </c>
       <c r="L21" t="n">
-        <v>17.56</v>
+        <v>18.03</v>
       </c>
       <c r="M21" s="2" t="n">
-        <v>94.2</v>
+        <v>93.97</v>
       </c>
       <c r="N21" s="2" t="n">
-        <v>98.42</v>
+        <v>98.34</v>
       </c>
       <c r="O21" t="n">
-        <v>20.03</v>
+        <v>25.44</v>
       </c>
       <c r="P21" t="n">
-        <v>10.57</v>
+        <v>12.89</v>
       </c>
       <c r="Q21" s="2" t="n">
-        <v>83.03</v>
+        <v>78.81</v>
       </c>
       <c r="R21" t="n">
-        <v>6.41</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="S21" t="inlineStr">
         <is>
@@ -2598,37 +2598,37 @@
         </is>
       </c>
       <c r="T21" s="2" t="n">
-        <v>93.59999999999999</v>
+        <v>91.7</v>
       </c>
       <c r="U21" t="n">
-        <v>16.98</v>
+        <v>21.19</v>
       </c>
       <c r="V21" s="2" t="n">
-        <v>89.44</v>
+        <v>87.11</v>
       </c>
       <c r="W21" t="n">
-        <v>17.91</v>
+        <v>22.38</v>
       </c>
       <c r="X21" s="2" t="n">
-        <v>98.09</v>
+        <v>97.29000000000001</v>
       </c>
       <c r="Y21" t="n">
-        <v>66.3</v>
+        <v>46.73</v>
       </c>
       <c r="Z21" t="n">
-        <v>29.51</v>
+        <v>56.24</v>
       </c>
       <c r="AA21" t="n">
-        <v>29.65</v>
+        <v>13.18</v>
       </c>
       <c r="AB21" t="n">
-        <v>4.86</v>
+        <v>20.08</v>
       </c>
       <c r="AC21" s="2" t="n">
-        <v>90.29000000000001</v>
+        <v>97.38</v>
       </c>
       <c r="AD21" s="2" t="n">
-        <v>99.45</v>
+        <v>94.87</v>
       </c>
     </row>
     <row r="22">
@@ -2639,98 +2639,98 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>APOEL</t>
+          <t>Borac</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Celje</t>
+          <t>Rapid</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>69.52</v>
+        <v>19.24</v>
       </c>
       <c r="E22" t="n">
-        <v>15.99</v>
+        <v>34.54</v>
       </c>
       <c r="F22" t="n">
-        <v>14.2</v>
+        <v>46.21</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2-1</t>
-        </is>
-      </c>
-      <c r="H22" s="2" t="n">
-        <v>85.50999999999999</v>
-      </c>
-      <c r="I22" s="2" t="n">
-        <v>83.72</v>
-      </c>
-      <c r="J22" t="n">
-        <v>30.19</v>
-      </c>
-      <c r="K22" s="2" t="n">
-        <v>92.09</v>
-      </c>
-      <c r="L22" s="2" t="n">
-        <v>78.45999999999999</v>
-      </c>
-      <c r="M22" t="n">
-        <v>39.85</v>
-      </c>
-      <c r="N22" t="n">
-        <v>59.3</v>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>53.78</v>
+      </c>
+      <c r="I22" t="n">
+        <v>65.45</v>
+      </c>
+      <c r="J22" s="2" t="n">
+        <v>80.75</v>
+      </c>
+      <c r="K22" t="n">
+        <v>41.44</v>
+      </c>
+      <c r="L22" t="n">
+        <v>17.64</v>
+      </c>
+      <c r="M22" s="2" t="n">
+        <v>94.16</v>
+      </c>
+      <c r="N22" s="2" t="n">
+        <v>98.41</v>
       </c>
       <c r="O22" t="n">
-        <v>68.68000000000001</v>
-      </c>
-      <c r="P22" s="2" t="n">
-        <v>73.55</v>
+        <v>23.02</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0</v>
       </c>
       <c r="Q22" t="n">
-        <v>22.18</v>
+        <v>57.9</v>
       </c>
       <c r="R22" t="n">
-        <v>1.67</v>
+        <v>42.07</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>1-0</t>
-        </is>
-      </c>
-      <c r="T22" s="2" t="n">
-        <v>95.72999999999999</v>
-      </c>
-      <c r="U22" s="2" t="n">
-        <v>75.22</v>
-      </c>
-      <c r="V22" t="n">
-        <v>23.85</v>
-      </c>
-      <c r="W22" s="2" t="n">
-        <v>79.48</v>
-      </c>
-      <c r="X22" t="n">
-        <v>46.74</v>
-      </c>
-      <c r="Y22" s="2" t="n">
-        <v>94.13</v>
-      </c>
-      <c r="Z22" s="2" t="n">
-        <v>72.44</v>
-      </c>
-      <c r="AA22" s="2" t="n">
-        <v>78.03</v>
+          <t>0-0</t>
+        </is>
+      </c>
+      <c r="T22" t="n">
+        <v>57.9</v>
+      </c>
+      <c r="U22" t="n">
+        <v>42.07</v>
+      </c>
+      <c r="V22" s="2" t="n">
+        <v>99.97</v>
+      </c>
+      <c r="W22" t="n">
+        <v>42.07</v>
+      </c>
+      <c r="X22" s="2" t="n">
+        <v>89.54000000000001</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>38.8</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>61.31</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>8.75</v>
       </c>
       <c r="AB22" t="n">
-        <v>37.09</v>
-      </c>
-      <c r="AC22" t="n">
-        <v>44.9</v>
+        <v>24.57</v>
+      </c>
+      <c r="AC22" s="2" t="n">
+        <v>98.63</v>
       </c>
       <c r="AD22" s="2" t="n">
-        <v>85.53</v>
+        <v>92.87</v>
       </c>
     </row>
     <row r="23">
@@ -2746,93 +2746,93 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>TSC</t>
-        </is>
-      </c>
-      <c r="D23" s="2" t="n">
-        <v>81.81</v>
+          <t>Cercle Brugge</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>65.15000000000001</v>
       </c>
       <c r="E23" t="n">
-        <v>12.17</v>
+        <v>20.12</v>
       </c>
       <c r="F23" t="n">
-        <v>5.7</v>
+        <v>14.72</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2-0</t>
+          <t>1-0</t>
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>93.98</v>
+        <v>85.27000000000001</v>
       </c>
       <c r="I23" s="2" t="n">
-        <v>87.51000000000001</v>
+        <v>79.87</v>
       </c>
       <c r="J23" t="n">
-        <v>17.87</v>
+        <v>34.84</v>
       </c>
       <c r="K23" s="2" t="n">
-        <v>87.45999999999999</v>
+        <v>72.90000000000001</v>
       </c>
       <c r="L23" t="n">
-        <v>69.53</v>
-      </c>
-      <c r="M23" t="n">
-        <v>51.37</v>
+        <v>48.6</v>
+      </c>
+      <c r="M23" s="2" t="n">
+        <v>73.2</v>
       </c>
       <c r="N23" s="2" t="n">
-        <v>70.51000000000001</v>
+        <v>87.48</v>
       </c>
       <c r="O23" t="n">
-        <v>47.24</v>
+        <v>43.55</v>
       </c>
       <c r="P23" t="n">
-        <v>55.39</v>
+        <v>14.44</v>
       </c>
       <c r="Q23" t="n">
-        <v>37.51</v>
+        <v>54.19</v>
       </c>
       <c r="R23" t="n">
-        <v>6.62</v>
+        <v>31.36</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
           <t>0-0</t>
         </is>
       </c>
-      <c r="T23" s="2" t="n">
-        <v>92.90000000000001</v>
+      <c r="T23" t="n">
+        <v>68.63</v>
       </c>
       <c r="U23" t="n">
-        <v>62.01</v>
-      </c>
-      <c r="V23" t="n">
-        <v>44.13</v>
-      </c>
-      <c r="W23" s="2" t="n">
-        <v>70.68000000000001</v>
-      </c>
-      <c r="X23" t="n">
-        <v>61.4</v>
+        <v>45.8</v>
+      </c>
+      <c r="V23" s="2" t="n">
+        <v>85.55</v>
+      </c>
+      <c r="W23" t="n">
+        <v>51.66</v>
+      </c>
+      <c r="X23" s="2" t="n">
+        <v>83.54000000000001</v>
       </c>
       <c r="Y23" s="2" t="n">
-        <v>94.28</v>
+        <v>84.72</v>
       </c>
       <c r="Z23" t="n">
-        <v>49.65</v>
-      </c>
-      <c r="AA23" s="2" t="n">
-        <v>78.5</v>
+        <v>52.23</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>56.02</v>
       </c>
       <c r="AB23" t="n">
-        <v>15.16</v>
-      </c>
-      <c r="AC23" t="n">
-        <v>44.19</v>
+        <v>16.94</v>
+      </c>
+      <c r="AC23" s="2" t="n">
+        <v>70.93000000000001</v>
       </c>
       <c r="AD23" s="2" t="n">
-        <v>96.41</v>
+        <v>96.08</v>
       </c>
     </row>
     <row r="24">
@@ -2843,98 +2843,98 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Panathinaikos</t>
+          <t>Celje</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Vikingur</t>
+          <t>Lugano</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>62.24</v>
+        <v>56.5</v>
       </c>
       <c r="E24" t="n">
-        <v>22.89</v>
+        <v>16.64</v>
       </c>
       <c r="F24" t="n">
-        <v>14.85</v>
+        <v>26.53</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
+          <t>2-2</t>
+        </is>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>73.14</v>
+      </c>
+      <c r="I24" s="2" t="n">
+        <v>83.03</v>
+      </c>
+      <c r="J24" t="n">
+        <v>43.17</v>
+      </c>
+      <c r="K24" s="2" t="n">
+        <v>95.06</v>
+      </c>
+      <c r="L24" s="2" t="n">
+        <v>86.54000000000001</v>
+      </c>
+      <c r="M24" t="n">
+        <v>27.6</v>
+      </c>
+      <c r="N24" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="O24" s="2" t="n">
+        <v>81.39</v>
+      </c>
+      <c r="P24" t="n">
+        <v>56.65</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>25.55</v>
+      </c>
+      <c r="R24" t="n">
+        <v>15.75</v>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
           <t>1-0</t>
         </is>
       </c>
-      <c r="H24" s="2" t="n">
-        <v>85.13</v>
-      </c>
-      <c r="I24" s="2" t="n">
-        <v>77.09</v>
-      </c>
-      <c r="J24" t="n">
-        <v>37.74</v>
-      </c>
-      <c r="K24" s="2" t="n">
-        <v>75.17</v>
-      </c>
-      <c r="L24" t="n">
-        <v>49.97</v>
-      </c>
-      <c r="M24" s="2" t="n">
-        <v>71.98999999999999</v>
-      </c>
-      <c r="N24" s="2" t="n">
+      <c r="T24" s="2" t="n">
+        <v>82.2</v>
+      </c>
+      <c r="U24" s="2" t="n">
+        <v>72.40000000000001</v>
+      </c>
+      <c r="V24" t="n">
+        <v>41.3</v>
+      </c>
+      <c r="W24" s="2" t="n">
         <v>86.68000000000001</v>
       </c>
-      <c r="O24" t="n">
-        <v>47.12</v>
-      </c>
-      <c r="P24" t="n">
-        <v>43.66</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>49.14</v>
-      </c>
-      <c r="R24" t="n">
-        <v>7.12</v>
-      </c>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>0-0</t>
-        </is>
-      </c>
-      <c r="T24" s="2" t="n">
-        <v>92.8</v>
-      </c>
-      <c r="U24" t="n">
-        <v>50.77999999999999</v>
-      </c>
-      <c r="V24" t="n">
-        <v>56.26</v>
-      </c>
-      <c r="W24" t="n">
-        <v>56.97</v>
-      </c>
-      <c r="X24" s="2" t="n">
-        <v>77.26000000000001</v>
+      <c r="X24" t="n">
+        <v>36.14</v>
       </c>
       <c r="Y24" s="2" t="n">
-        <v>84.64</v>
-      </c>
-      <c r="Z24" t="n">
-        <v>55.04</v>
-      </c>
-      <c r="AA24" t="n">
-        <v>55.87</v>
+        <v>94.18000000000001</v>
+      </c>
+      <c r="Z24" s="2" t="n">
+        <v>86.45</v>
+      </c>
+      <c r="AA24" s="2" t="n">
+        <v>78.26000000000001</v>
       </c>
       <c r="AB24" t="n">
-        <v>19.1</v>
-      </c>
-      <c r="AC24" s="2" t="n">
-        <v>71.06999999999999</v>
-      </c>
-      <c r="AD24" s="2" t="n">
-        <v>95.25</v>
+        <v>59.74</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>44.52</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>66.91</v>
       </c>
     </row>
     <row r="25">
@@ -2945,98 +2945,98 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Shamrock</t>
+          <t>Pafos</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Molde</t>
-        </is>
-      </c>
-      <c r="D25" s="2" t="n">
-        <v>88.86</v>
+          <t>Djurgarden</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>53.89</v>
       </c>
       <c r="E25" t="n">
-        <v>5.92</v>
+        <v>20.84</v>
       </c>
       <c r="F25" t="n">
-        <v>2.61</v>
+        <v>25.25</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>4-0</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="H25" s="2" t="n">
-        <v>94.78</v>
+        <v>74.73</v>
       </c>
       <c r="I25" s="2" t="n">
-        <v>91.47</v>
+        <v>79.14</v>
       </c>
       <c r="J25" t="n">
-        <v>8.529999999999999</v>
+        <v>46.09</v>
       </c>
       <c r="K25" s="2" t="n">
-        <v>93.14</v>
-      </c>
-      <c r="L25" s="2" t="n">
-        <v>84.12</v>
+        <v>81.5</v>
+      </c>
+      <c r="L25" t="n">
+        <v>60.94</v>
       </c>
       <c r="M25" t="n">
-        <v>27.83</v>
-      </c>
-      <c r="N25" t="n">
-        <v>45.69</v>
+        <v>61.36</v>
+      </c>
+      <c r="N25" s="2" t="n">
+        <v>78.94</v>
       </c>
       <c r="O25" t="n">
-        <v>51.07</v>
+        <v>59.77</v>
       </c>
       <c r="P25" t="n">
-        <v>69.31</v>
+        <v>15.08</v>
       </c>
       <c r="Q25" t="n">
-        <v>7.12</v>
+        <v>48.88</v>
       </c>
       <c r="R25" t="n">
-        <v>0.73</v>
+        <v>36.01</v>
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>3-0</t>
-        </is>
-      </c>
-      <c r="T25" s="2" t="n">
-        <v>76.43000000000001</v>
-      </c>
-      <c r="U25" s="2" t="n">
-        <v>70.04000000000001</v>
-      </c>
-      <c r="V25" t="n">
-        <v>7.85</v>
-      </c>
-      <c r="W25" s="2" t="n">
-        <v>73.63</v>
-      </c>
-      <c r="X25" t="n">
-        <v>13.01</v>
+          <t>0-0</t>
+        </is>
+      </c>
+      <c r="T25" t="n">
+        <v>63.96</v>
+      </c>
+      <c r="U25" t="n">
+        <v>51.09</v>
+      </c>
+      <c r="V25" s="2" t="n">
+        <v>84.89</v>
+      </c>
+      <c r="W25" t="n">
+        <v>58.39</v>
+      </c>
+      <c r="X25" s="2" t="n">
+        <v>78.16</v>
       </c>
       <c r="Y25" s="2" t="n">
-        <v>95.81</v>
-      </c>
-      <c r="Z25" t="n">
-        <v>51.79</v>
-      </c>
-      <c r="AA25" s="2" t="n">
-        <v>89.26000000000001</v>
+        <v>85.23</v>
+      </c>
+      <c r="Z25" s="2" t="n">
+        <v>70.94</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>57</v>
       </c>
       <c r="AB25" t="n">
-        <v>17.19</v>
+        <v>35.03</v>
       </c>
       <c r="AC25" t="n">
-        <v>21.72</v>
+        <v>69.98999999999999</v>
       </c>
       <c r="AD25" s="2" t="n">
-        <v>93.33</v>
+        <v>87.14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated until 23.03.2025 and deleted day files
</commit_message>
<xml_diff>
--- a/UEFA.xlsx
+++ b/UEFA.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD13"/>
+  <dimension ref="A1:AD19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -599,98 +599,98 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>Croatia</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>France</t>
-        </is>
-      </c>
       <c r="D2" t="n">
-        <v>4.28</v>
+        <v>26.51</v>
       </c>
       <c r="E2" t="n">
-        <v>14</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>81.58</v>
+        <v>30.74</v>
+      </c>
+      <c r="F2" t="n">
+        <v>42.75</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0-2</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>18.28</v>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>85.86</v>
+        <v>57.25</v>
+      </c>
+      <c r="I2" t="n">
+        <v>69.26000000000001</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>95.58</v>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>82.09999999999999</v>
+        <v>73.48999999999999</v>
+      </c>
+      <c r="K2" t="n">
+        <v>68.31</v>
       </c>
       <c r="L2" t="n">
-        <v>59.7</v>
-      </c>
-      <c r="M2" t="n">
-        <v>62.52</v>
+        <v>40.36</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>79.95999999999999</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>79.84999999999999</v>
+        <v>91.64</v>
       </c>
       <c r="O2" t="n">
-        <v>36.92</v>
+        <v>47.23</v>
       </c>
       <c r="P2" t="n">
-        <v>-0</v>
+        <v>37.99</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>37.96</v>
       </c>
       <c r="R2" t="n">
-        <v>0.45</v>
+        <v>20.2</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>0-4</t>
-        </is>
-      </c>
-      <c r="T2" t="n">
-        <v>0</v>
+          <t>1-1</t>
+        </is>
+      </c>
+      <c r="T2" s="2" t="n">
+        <v>75.95</v>
       </c>
       <c r="U2" t="n">
-        <v>0.45</v>
+        <v>58.19</v>
       </c>
       <c r="V2" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0.45</v>
+        <v>58.16</v>
+      </c>
+      <c r="W2" s="2" t="n">
+        <v>83.86</v>
       </c>
       <c r="X2" t="n">
-        <v>0</v>
+        <v>13.62</v>
       </c>
       <c r="Y2" t="n">
-        <v>39.08</v>
+        <v>62.62</v>
       </c>
       <c r="Z2" s="2" t="n">
-        <v>92.44</v>
+        <v>73.13</v>
       </c>
       <c r="AA2" t="n">
-        <v>8.9</v>
-      </c>
-      <c r="AB2" s="2" t="n">
-        <v>73.15000000000001</v>
+        <v>25.84</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>37.82</v>
       </c>
       <c r="AC2" s="2" t="n">
-        <v>98.44</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>51.8</v>
+        <v>92.26000000000001</v>
+      </c>
+      <c r="AD2" s="2" t="n">
+        <v>85.38</v>
       </c>
     </row>
     <row r="3">
@@ -701,98 +701,98 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Portugal</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>27.87</v>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>91.27</v>
       </c>
       <c r="E3" t="n">
-        <v>37.43</v>
+        <v>3.45</v>
       </c>
       <c r="F3" t="n">
-        <v>34.69</v>
+        <v>0.88</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>4-0</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>94.72</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>92.14999999999999</v>
+      </c>
+      <c r="J3" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>91.98999999999999</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>83.83</v>
+      </c>
+      <c r="M3" t="n">
+        <v>25.34</v>
+      </c>
+      <c r="N3" t="n">
+        <v>42.58</v>
+      </c>
+      <c r="O3" t="n">
+        <v>37.72</v>
+      </c>
+      <c r="P3" t="n">
+        <v>21.27</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>55.53</v>
+      </c>
+      <c r="R3" t="n">
+        <v>23.12</v>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
           <t>0-0</t>
         </is>
       </c>
-      <c r="H3" t="n">
-        <v>65.3</v>
-      </c>
-      <c r="I3" t="n">
-        <v>62.56</v>
-      </c>
-      <c r="J3" s="2" t="n">
-        <v>72.12</v>
-      </c>
-      <c r="K3" t="n">
-        <v>51.93</v>
-      </c>
-      <c r="L3" t="n">
-        <v>23.94</v>
-      </c>
-      <c r="M3" s="2" t="n">
-        <v>90.87</v>
-      </c>
-      <c r="N3" s="2" t="n">
-        <v>97.12</v>
-      </c>
-      <c r="O3" t="n">
-        <v>33.97</v>
-      </c>
-      <c r="P3" t="n">
-        <v>7.01</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>58.37</v>
-      </c>
-      <c r="R3" t="n">
-        <v>34.6</v>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>0-0</t>
-        </is>
-      </c>
-      <c r="T3" t="n">
-        <v>65.38</v>
+      <c r="T3" s="2" t="n">
+        <v>76.8</v>
       </c>
       <c r="U3" t="n">
-        <v>41.61</v>
+        <v>44.39</v>
       </c>
       <c r="V3" s="2" t="n">
-        <v>92.97</v>
+        <v>78.65000000000001</v>
       </c>
       <c r="W3" t="n">
-        <v>48.12</v>
-      </c>
-      <c r="X3" s="2" t="n">
-        <v>82.38</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>54.28</v>
+        <v>63.38</v>
+      </c>
+      <c r="X3" t="n">
+        <v>58.65</v>
+      </c>
+      <c r="Y3" s="2" t="n">
+        <v>94.56999999999999</v>
       </c>
       <c r="Z3" t="n">
-        <v>59.52</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>18.5</v>
+        <v>37.98</v>
+      </c>
+      <c r="AA3" s="2" t="n">
+        <v>89.87</v>
       </c>
       <c r="AB3" t="n">
-        <v>22.91</v>
-      </c>
-      <c r="AC3" s="2" t="n">
-        <v>95.5</v>
+        <v>8.800000000000001</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>16.5</v>
       </c>
       <c r="AD3" s="2" t="n">
-        <v>93.64</v>
+        <v>94.18000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -803,98 +803,98 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Denmark</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>23.47</v>
+        <v>26.77</v>
       </c>
       <c r="E4" t="n">
-        <v>22.39</v>
+        <v>38.72</v>
       </c>
       <c r="F4" t="n">
-        <v>54.09</v>
+        <v>34.51</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>0-0</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>45.86</v>
-      </c>
-      <c r="I4" s="2" t="n">
-        <v>77.56</v>
+        <v>65.48999999999999</v>
+      </c>
+      <c r="I4" t="n">
+        <v>61.28</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>76.48</v>
-      </c>
-      <c r="K4" s="2" t="n">
-        <v>88.87</v>
-      </c>
-      <c r="L4" s="2" t="n">
-        <v>70.47</v>
-      </c>
-      <c r="M4" t="n">
-        <v>50.56</v>
-      </c>
-      <c r="N4" t="n">
-        <v>69.77</v>
+        <v>73.22999999999999</v>
+      </c>
+      <c r="K4" t="n">
+        <v>47.15</v>
+      </c>
+      <c r="L4" t="n">
+        <v>20.29</v>
+      </c>
+      <c r="M4" s="2" t="n">
+        <v>92.84</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <v>97.92</v>
       </c>
       <c r="O4" t="n">
-        <v>68.83</v>
+        <v>30.18</v>
       </c>
       <c r="P4" t="n">
-        <v>11.6</v>
+        <v>41.46</v>
       </c>
       <c r="Q4" t="n">
-        <v>44.75</v>
+        <v>55.58</v>
       </c>
       <c r="R4" t="n">
-        <v>43.18</v>
+        <v>2.92</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
           <t>0-0</t>
         </is>
       </c>
-      <c r="T4" t="n">
-        <v>56.35</v>
+      <c r="T4" s="2" t="n">
+        <v>97.03999999999999</v>
       </c>
       <c r="U4" t="n">
-        <v>54.78</v>
-      </c>
-      <c r="V4" s="2" t="n">
-        <v>87.93000000000001</v>
-      </c>
-      <c r="W4" s="2" t="n">
-        <v>72.64</v>
-      </c>
-      <c r="X4" t="n">
-        <v>49.25</v>
-      </c>
-      <c r="Y4" s="2" t="n">
-        <v>76.12</v>
-      </c>
-      <c r="Z4" s="2" t="n">
-        <v>89</v>
+        <v>44.38</v>
+      </c>
+      <c r="V4" t="n">
+        <v>58.5</v>
+      </c>
+      <c r="W4" t="n">
+        <v>48.72</v>
+      </c>
+      <c r="X4" s="2" t="n">
+        <v>82.68000000000001</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>50.66</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>56.83</v>
       </c>
       <c r="AA4" t="n">
-        <v>41.96</v>
+        <v>15.8</v>
       </c>
       <c r="AB4" t="n">
-        <v>64.78</v>
+        <v>20.57</v>
       </c>
       <c r="AC4" s="2" t="n">
-        <v>82.48</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>61.96</v>
+        <v>96.51000000000001</v>
+      </c>
+      <c r="AD4" s="2" t="n">
+        <v>94.66</v>
       </c>
     </row>
     <row r="5">
@@ -905,98 +905,98 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>Spain</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>Netherlands</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Spain</t>
-        </is>
-      </c>
       <c r="D5" s="2" t="n">
-        <v>80.47</v>
+        <v>74.26000000000001</v>
       </c>
       <c r="E5" t="n">
-        <v>13.38</v>
+        <v>15.6</v>
       </c>
       <c r="F5" t="n">
-        <v>5.83</v>
+        <v>9.880000000000001</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2-0</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="H5" s="2" t="n">
-        <v>93.84999999999999</v>
+        <v>89.86</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>86.3</v>
+        <v>84.14</v>
       </c>
       <c r="J5" t="n">
-        <v>19.21</v>
+        <v>25.48</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>88.31</v>
+        <v>90.08</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>70.29000000000001</v>
+        <v>73.63</v>
       </c>
       <c r="M5" t="n">
-        <v>50.46</v>
+        <v>46.34</v>
       </c>
       <c r="N5" t="n">
-        <v>69.68000000000001</v>
+        <v>65.81999999999999</v>
       </c>
       <c r="O5" t="n">
-        <v>49.79</v>
-      </c>
-      <c r="P5" s="2" t="n">
-        <v>77.7</v>
+        <v>60.29</v>
+      </c>
+      <c r="P5" t="n">
+        <v>46.45</v>
       </c>
       <c r="Q5" t="n">
-        <v>11.13</v>
+        <v>45.46</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.02</v>
+        <v>7.48</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>2-0</t>
+          <t>0-0</t>
         </is>
       </c>
       <c r="T5" s="2" t="n">
-        <v>88.83</v>
-      </c>
-      <c r="U5" s="2" t="n">
-        <v>77.68000000000001</v>
+        <v>91.91</v>
+      </c>
+      <c r="U5" t="n">
+        <v>53.93000000000001</v>
       </c>
       <c r="V5" t="n">
-        <v>11.11</v>
+        <v>52.94</v>
       </c>
       <c r="W5" s="2" t="n">
-        <v>80.65000000000001</v>
+        <v>71.84</v>
       </c>
       <c r="X5" t="n">
-        <v>25.27</v>
+        <v>47.47</v>
       </c>
       <c r="Y5" s="2" t="n">
-        <v>94.26000000000001</v>
+        <v>93.90000000000001</v>
       </c>
       <c r="Z5" t="n">
-        <v>51.9</v>
+        <v>63.32</v>
       </c>
       <c r="AA5" s="2" t="n">
-        <v>78.45999999999999</v>
+        <v>77.33</v>
       </c>
       <c r="AB5" t="n">
-        <v>16.77</v>
+        <v>26.63</v>
       </c>
       <c r="AC5" t="n">
-        <v>44.25</v>
+        <v>45.95</v>
       </c>
       <c r="AD5" s="2" t="n">
-        <v>95.84</v>
+        <v>91.58</v>
       </c>
     </row>
     <row r="6">
@@ -1007,98 +1007,98 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>Armenia</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Georgia</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>5.23</v>
+      <c r="D6" s="2" t="n">
+        <v>91.26000000000001</v>
       </c>
       <c r="E6" t="n">
-        <v>12.8</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>81.64</v>
+        <v>5.74</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.42</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0-2</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>18.03</v>
+          <t>3-0</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>97</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>86.87</v>
-      </c>
-      <c r="J6" s="2" t="n">
-        <v>94.44</v>
+        <v>92.68000000000001</v>
+      </c>
+      <c r="J6" t="n">
+        <v>7.16</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>88.17</v>
+        <v>91.19</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>70.11</v>
+        <v>78.01000000000001</v>
       </c>
       <c r="M6" t="n">
-        <v>50.65</v>
+        <v>38.68</v>
       </c>
       <c r="N6" t="n">
-        <v>69.86</v>
+        <v>58.07</v>
       </c>
       <c r="O6" t="n">
-        <v>47.93</v>
-      </c>
-      <c r="P6" t="n">
-        <v>-0</v>
+        <v>35.45</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>70.5</v>
       </c>
       <c r="Q6" t="n">
-        <v>0</v>
+        <v>26.03</v>
       </c>
       <c r="R6" t="n">
-        <v>0.05</v>
+        <v>0.48</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>0-4</t>
-        </is>
-      </c>
-      <c r="T6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" t="n">
-        <v>0.05</v>
+          <t>1-0</t>
+        </is>
+      </c>
+      <c r="T6" s="2" t="n">
+        <v>96.53</v>
+      </c>
+      <c r="U6" s="2" t="n">
+        <v>70.98</v>
       </c>
       <c r="V6" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="W6" t="n">
-        <v>0.05</v>
+        <v>26.51</v>
+      </c>
+      <c r="W6" s="2" t="n">
+        <v>78.84</v>
       </c>
       <c r="X6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>49.88</v>
-      </c>
-      <c r="Z6" s="2" t="n">
-        <v>94.41</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>15.32</v>
-      </c>
-      <c r="AB6" s="2" t="n">
-        <v>78.94</v>
-      </c>
-      <c r="AC6" s="2" t="n">
-        <v>96.33</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>43.52</v>
+        <v>41.04</v>
+      </c>
+      <c r="Y6" s="2" t="n">
+        <v>96.17</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>36.01</v>
+      </c>
+      <c r="AA6" s="2" t="n">
+        <v>87.61</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>7.58</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>27.03</v>
+      </c>
+      <c r="AD6" s="2" t="n">
+        <v>97.31999999999999</v>
       </c>
     </row>
     <row r="7">
@@ -1109,98 +1109,98 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>Hungary</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>Turkiye</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Hungary</t>
-        </is>
-      </c>
       <c r="D7" t="n">
-        <v>7.36</v>
+        <v>29.83</v>
       </c>
       <c r="E7" t="n">
-        <v>24.78</v>
+        <v>32.08</v>
       </c>
       <c r="F7" t="n">
-        <v>67.86</v>
+        <v>38.09</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>32.14</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <v>75.22</v>
+        <v>61.91</v>
+      </c>
+      <c r="I7" t="n">
+        <v>67.92</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>92.64</v>
+        <v>70.17</v>
       </c>
       <c r="K7" t="n">
-        <v>62.28</v>
+        <v>65.56</v>
       </c>
       <c r="L7" t="n">
-        <v>34.17</v>
+        <v>37.23</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>84.45999999999999</v>
+        <v>82.3</v>
       </c>
       <c r="N7" s="2" t="n">
-        <v>94.09999999999999</v>
+        <v>92.95</v>
       </c>
       <c r="O7" t="n">
-        <v>27.92</v>
+        <v>45.34</v>
       </c>
       <c r="P7" t="n">
-        <v>-0</v>
+        <v>51.47</v>
       </c>
       <c r="Q7" t="n">
-        <v>0</v>
+        <v>45.62</v>
       </c>
       <c r="R7" t="n">
-        <v>2.67</v>
+        <v>2.68</v>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>0-4</t>
-        </is>
-      </c>
-      <c r="T7" t="n">
-        <v>0</v>
+          <t>0-0</t>
+        </is>
+      </c>
+      <c r="T7" s="2" t="n">
+        <v>97.09</v>
       </c>
       <c r="U7" t="n">
-        <v>2.67</v>
+        <v>54.15</v>
       </c>
       <c r="V7" t="n">
-        <v>2.67</v>
+        <v>48.3</v>
       </c>
       <c r="W7" t="n">
-        <v>2.67</v>
-      </c>
-      <c r="X7" t="n">
-        <v>0.04</v>
+        <v>61.18</v>
+      </c>
+      <c r="X7" s="2" t="n">
+        <v>70.01000000000001</v>
       </c>
       <c r="Y7" t="n">
-        <v>33.1</v>
-      </c>
-      <c r="Z7" s="2" t="n">
-        <v>81.09999999999999</v>
+        <v>63.54</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>69.04000000000001</v>
       </c>
       <c r="AA7" t="n">
-        <v>6.21</v>
+        <v>26.75</v>
       </c>
       <c r="AB7" t="n">
-        <v>49.62</v>
+        <v>32.74</v>
       </c>
       <c r="AC7" s="2" t="n">
-        <v>99.19</v>
+        <v>91.8</v>
       </c>
       <c r="AD7" s="2" t="n">
-        <v>76.61</v>
+        <v>88.54000000000001</v>
       </c>
     </row>
     <row r="8">
@@ -1211,98 +1211,98 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Austria</t>
+          <t>Iceland</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Serbia</t>
+          <t>Kosovo</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>53.92</v>
+        <v>44.68</v>
       </c>
       <c r="E8" t="n">
-        <v>0.03</v>
+        <v>24.89</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>30.42</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>8-0</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>53.95</v>
-      </c>
-      <c r="I8" t="n">
-        <v>53.92</v>
+        <v>69.56999999999999</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>75.09999999999999</v>
       </c>
       <c r="J8" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="K8" t="n">
-        <v>53.75</v>
+        <v>55.31</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>85.17</v>
       </c>
       <c r="L8" t="n">
-        <v>52.97</v>
+        <v>63.97</v>
       </c>
       <c r="M8" t="n">
-        <v>3.16</v>
-      </c>
-      <c r="N8" t="n">
-        <v>7.75</v>
+        <v>58.12</v>
+      </c>
+      <c r="N8" s="2" t="n">
+        <v>76.33</v>
       </c>
       <c r="O8" t="n">
-        <v>2.65</v>
+        <v>65.75</v>
       </c>
       <c r="P8" t="n">
-        <v>29.36</v>
+        <v>30.14</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.3</v>
+        <v>55.19</v>
       </c>
       <c r="R8" t="n">
-        <v>-0</v>
+        <v>14.58</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>4-0</t>
-        </is>
-      </c>
-      <c r="T8" t="n">
-        <v>29.66</v>
+          <t>0-0</t>
+        </is>
+      </c>
+      <c r="T8" s="2" t="n">
+        <v>85.33</v>
       </c>
       <c r="U8" t="n">
-        <v>29.36</v>
+        <v>44.72</v>
       </c>
       <c r="V8" t="n">
-        <v>0.3</v>
+        <v>69.77</v>
       </c>
       <c r="W8" t="n">
-        <v>29.37</v>
+        <v>61.86</v>
       </c>
       <c r="X8" t="n">
-        <v>1.84</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>53.93</v>
-      </c>
-      <c r="Z8" t="n">
-        <v>2.65</v>
+        <v>61.79</v>
+      </c>
+      <c r="Y8" s="2" t="n">
+        <v>83.75</v>
+      </c>
+      <c r="Z8" s="2" t="n">
+        <v>77.18000000000001</v>
       </c>
       <c r="AA8" t="n">
-        <v>53.74</v>
+        <v>54.24</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>1.02</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>53.95</v>
+        <v>43.48</v>
+      </c>
+      <c r="AC8" s="2" t="n">
+        <v>72.58</v>
+      </c>
+      <c r="AD8" s="2" t="n">
+        <v>81.42</v>
       </c>
     </row>
     <row r="9">
@@ -1313,98 +1313,98 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Bulgaria</t>
+          <t>Scotland</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>42.72</v>
+        <v>53.86</v>
       </c>
       <c r="E9" t="n">
-        <v>40.41</v>
+        <v>31.76</v>
       </c>
       <c r="F9" t="n">
-        <v>16.87</v>
+        <v>14.38</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
+          <t>1-0</t>
+        </is>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>85.62</v>
+      </c>
+      <c r="I9" t="n">
+        <v>68.23999999999999</v>
+      </c>
+      <c r="J9" t="n">
+        <v>46.14</v>
+      </c>
+      <c r="K9" t="n">
+        <v>55.93</v>
+      </c>
+      <c r="L9" t="n">
+        <v>27.83</v>
+      </c>
+      <c r="M9" s="2" t="n">
+        <v>88.59</v>
+      </c>
+      <c r="N9" s="2" t="n">
+        <v>96.11</v>
+      </c>
+      <c r="O9" t="n">
+        <v>31.58</v>
+      </c>
+      <c r="P9" t="n">
+        <v>54.73</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>43.59</v>
+      </c>
+      <c r="R9" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
           <t>0-0</t>
         </is>
       </c>
-      <c r="H9" s="2" t="n">
-        <v>83.13</v>
-      </c>
-      <c r="I9" t="n">
-        <v>59.59</v>
-      </c>
-      <c r="J9" t="n">
-        <v>57.28</v>
-      </c>
-      <c r="K9" t="n">
-        <v>40.34</v>
-      </c>
-      <c r="L9" t="n">
-        <v>15.4</v>
-      </c>
-      <c r="M9" s="2" t="n">
-        <v>95.2</v>
-      </c>
-      <c r="N9" s="2" t="n">
-        <v>98.77</v>
-      </c>
-      <c r="O9" t="n">
-        <v>23.03</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" t="n">
-        <v>-0</v>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>4-0</t>
-        </is>
-      </c>
-      <c r="T9" t="n">
-        <v>0</v>
+      <c r="T9" s="2" t="n">
+        <v>98.31999999999999</v>
       </c>
       <c r="U9" t="n">
-        <v>0</v>
+        <v>56.16999999999999</v>
       </c>
       <c r="V9" t="n">
-        <v>0</v>
+        <v>45.03</v>
       </c>
       <c r="W9" t="n">
-        <v>0</v>
-      </c>
-      <c r="X9" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y9" t="n">
-        <v>58.85</v>
+        <v>60.44</v>
+      </c>
+      <c r="X9" s="2" t="n">
+        <v>72.83</v>
+      </c>
+      <c r="Y9" s="2" t="n">
+        <v>72.5</v>
       </c>
       <c r="Z9" t="n">
-        <v>36.85</v>
+        <v>41.86</v>
       </c>
       <c r="AA9" t="n">
-        <v>22.31</v>
+        <v>37</v>
       </c>
       <c r="AB9" t="n">
-        <v>7.82</v>
+        <v>10.33</v>
       </c>
       <c r="AC9" s="2" t="n">
-        <v>93.91</v>
+        <v>85.92</v>
       </c>
       <c r="AD9" s="2" t="n">
-        <v>98.84999999999999</v>
+        <v>98.22</v>
       </c>
     </row>
     <row r="10">
@@ -1415,98 +1415,98 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Serbia</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Scotland</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>93.5</v>
+          <t>Austria</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>38.54</v>
       </c>
       <c r="E10" t="n">
-        <v>4.79</v>
+        <v>38.48</v>
       </c>
       <c r="F10" t="n">
-        <v>0.5600000000000001</v>
+        <v>22.99</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>3-0</t>
+          <t>0-0</t>
         </is>
       </c>
       <c r="H10" s="2" t="n">
-        <v>98.29000000000001</v>
-      </c>
-      <c r="I10" s="2" t="n">
-        <v>94.06</v>
+        <v>77.02</v>
+      </c>
+      <c r="I10" t="n">
+        <v>61.53</v>
       </c>
       <c r="J10" t="n">
-        <v>5.35</v>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>88.44</v>
-      </c>
-      <c r="L10" s="2" t="n">
-        <v>72.16</v>
-      </c>
-      <c r="M10" t="n">
-        <v>47.09</v>
-      </c>
-      <c r="N10" t="n">
-        <v>66.54000000000001</v>
+        <v>61.47</v>
+      </c>
+      <c r="K10" t="n">
+        <v>46.6</v>
+      </c>
+      <c r="L10" t="n">
+        <v>19.9</v>
+      </c>
+      <c r="M10" s="2" t="n">
+        <v>93.04000000000001</v>
+      </c>
+      <c r="N10" s="2" t="n">
+        <v>97.98999999999999</v>
       </c>
       <c r="O10" t="n">
-        <v>19.26</v>
+        <v>29.13</v>
       </c>
       <c r="P10" t="n">
-        <v>6.75</v>
+        <v>0.89</v>
       </c>
       <c r="Q10" t="n">
-        <v>67.90000000000001</v>
+        <v>43.44</v>
       </c>
       <c r="R10" t="n">
-        <v>25.35</v>
+        <v>55.46</v>
       </c>
       <c r="S10" t="inlineStr">
         <is>
           <t>0-0</t>
         </is>
       </c>
-      <c r="T10" s="2" t="n">
-        <v>74.65000000000001</v>
+      <c r="T10" t="n">
+        <v>44.33</v>
       </c>
       <c r="U10" t="n">
-        <v>32.1</v>
+        <v>56.35</v>
       </c>
       <c r="V10" s="2" t="n">
-        <v>93.25</v>
+        <v>98.90000000000001</v>
       </c>
       <c r="W10" t="n">
-        <v>35.95</v>
+        <v>58.99</v>
       </c>
       <c r="X10" s="2" t="n">
-        <v>90.76000000000001</v>
-      </c>
-      <c r="Y10" s="2" t="n">
-        <v>96.09</v>
+        <v>75.44</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>59.33</v>
       </c>
       <c r="Z10" t="n">
-        <v>19.59</v>
-      </c>
-      <c r="AA10" s="2" t="n">
-        <v>86.2</v>
+        <v>46.82</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>22.74</v>
       </c>
       <c r="AB10" t="n">
-        <v>2.08</v>
-      </c>
-      <c r="AC10" t="n">
-        <v>30.42</v>
+        <v>13.24</v>
+      </c>
+      <c r="AC10" s="2" t="n">
+        <v>93.72</v>
       </c>
       <c r="AD10" s="2" t="n">
-        <v>98.7</v>
+        <v>97.37</v>
       </c>
     </row>
     <row r="11">
@@ -1517,98 +1517,98 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Kosovo</t>
+          <t>Slovenia</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Iceland</t>
-        </is>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>78.26000000000001</v>
+          <t>Slovakia</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>44.83</v>
       </c>
       <c r="E11" t="n">
-        <v>0.92</v>
+        <v>37.31</v>
       </c>
       <c r="F11" t="n">
-        <v>0.22</v>
+        <v>17.86</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>6-0</t>
+          <t>0-0</t>
         </is>
       </c>
       <c r="H11" s="2" t="n">
-        <v>79.18000000000001</v>
-      </c>
-      <c r="I11" s="2" t="n">
-        <v>78.48</v>
+        <v>82.14</v>
+      </c>
+      <c r="I11" t="n">
+        <v>62.69</v>
       </c>
       <c r="J11" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="K11" s="2" t="n">
-        <v>78.73</v>
-      </c>
-      <c r="L11" s="2" t="n">
-        <v>76.51000000000001</v>
-      </c>
-      <c r="M11" t="n">
-        <v>7.99</v>
-      </c>
-      <c r="N11" t="n">
-        <v>16.97</v>
+        <v>55.17</v>
+      </c>
+      <c r="K11" t="n">
+        <v>46.38</v>
+      </c>
+      <c r="L11" t="n">
+        <v>19.79</v>
+      </c>
+      <c r="M11" s="2" t="n">
+        <v>93.09</v>
+      </c>
+      <c r="N11" s="2" t="n">
+        <v>98.01000000000001</v>
       </c>
       <c r="O11" t="n">
-        <v>33.87</v>
+        <v>27.2</v>
       </c>
       <c r="P11" t="n">
-        <v>34.22</v>
+        <v>30.51</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.5</v>
+        <v>56.44</v>
       </c>
       <c r="R11" t="n">
-        <v>-0.02</v>
+        <v>13</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>4-0</t>
-        </is>
-      </c>
-      <c r="T11" t="n">
-        <v>34.72</v>
+          <t>0-0</t>
+        </is>
+      </c>
+      <c r="T11" s="2" t="n">
+        <v>86.95</v>
       </c>
       <c r="U11" t="n">
-        <v>34.2</v>
+        <v>43.51000000000001</v>
       </c>
       <c r="V11" t="n">
-        <v>0.48</v>
+        <v>69.44</v>
       </c>
       <c r="W11" t="n">
-        <v>34.3</v>
+        <v>58.41</v>
       </c>
       <c r="X11" t="n">
-        <v>2.41</v>
-      </c>
-      <c r="Y11" s="2" t="n">
-        <v>79.23999999999999</v>
+        <v>67.17</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>63.13</v>
       </c>
       <c r="Z11" t="n">
-        <v>33.9</v>
-      </c>
-      <c r="AA11" s="2" t="n">
-        <v>78.25</v>
+        <v>41.09</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>26.34</v>
       </c>
       <c r="AB11" t="n">
-        <v>8.57</v>
-      </c>
-      <c r="AC11" t="n">
-        <v>4.37</v>
+        <v>9.92</v>
+      </c>
+      <c r="AC11" s="2" t="n">
+        <v>92.01000000000001</v>
       </c>
       <c r="AD11" s="2" t="n">
-        <v>77.88</v>
+        <v>98.33</v>
       </c>
     </row>
     <row r="12">
@@ -1619,98 +1619,98 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Slovakia</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Slovenia</t>
+          <t>Ukraine</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>16.76</v>
+        <v>28.22</v>
       </c>
       <c r="E12" t="n">
-        <v>30.63</v>
+        <v>27.48</v>
       </c>
       <c r="F12" t="n">
-        <v>52.6</v>
+        <v>44.3</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>47.39</v>
-      </c>
-      <c r="I12" t="n">
-        <v>69.36</v>
+        <v>55.7</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>72.52</v>
       </c>
       <c r="J12" s="2" t="n">
-        <v>83.23</v>
-      </c>
-      <c r="K12" t="n">
-        <v>62.96</v>
+        <v>71.78</v>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>77.97</v>
       </c>
       <c r="L12" t="n">
-        <v>34.43</v>
-      </c>
-      <c r="M12" s="2" t="n">
-        <v>84.29000000000001</v>
+        <v>52.76</v>
+      </c>
+      <c r="M12" t="n">
+        <v>69.47</v>
       </c>
       <c r="N12" s="2" t="n">
-        <v>94.01000000000001</v>
+        <v>84.95999999999999</v>
       </c>
       <c r="O12" t="n">
-        <v>38.72</v>
+        <v>57.04</v>
       </c>
       <c r="P12" t="n">
-        <v>12.58</v>
+        <v>55.28</v>
       </c>
       <c r="Q12" t="n">
-        <v>47.42</v>
+        <v>40.12</v>
       </c>
       <c r="R12" t="n">
-        <v>39.74</v>
+        <v>3.71</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
           <t>0-0</t>
         </is>
       </c>
-      <c r="T12" t="n">
-        <v>60</v>
+      <c r="T12" s="2" t="n">
+        <v>95.40000000000001</v>
       </c>
       <c r="U12" t="n">
-        <v>52.32</v>
-      </c>
-      <c r="V12" s="2" t="n">
-        <v>87.16</v>
-      </c>
-      <c r="W12" t="n">
-        <v>69.3</v>
+        <v>58.99</v>
+      </c>
+      <c r="V12" t="n">
+        <v>43.83</v>
+      </c>
+      <c r="W12" s="2" t="n">
+        <v>72.56</v>
       </c>
       <c r="X12" t="n">
-        <v>54.83</v>
-      </c>
-      <c r="Y12" t="n">
-        <v>49.47</v>
+        <v>49.68</v>
+      </c>
+      <c r="Y12" s="2" t="n">
+        <v>70.36</v>
       </c>
       <c r="Z12" s="2" t="n">
-        <v>75.20999999999999</v>
+        <v>79.23</v>
       </c>
       <c r="AA12" t="n">
-        <v>14.98</v>
+        <v>34.31</v>
       </c>
       <c r="AB12" t="n">
-        <v>40.64</v>
+        <v>46.59</v>
       </c>
       <c r="AC12" s="2" t="n">
-        <v>96.79000000000001</v>
+        <v>87.59999999999999</v>
       </c>
       <c r="AD12" s="2" t="n">
-        <v>83.47</v>
+        <v>79.06</v>
       </c>
     </row>
     <row r="13">
@@ -1721,98 +1721,710 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Bulgaria</t>
         </is>
       </c>
       <c r="D13" s="2" t="n">
-        <v>89.15000000000001</v>
+        <v>77.73</v>
       </c>
       <c r="E13" t="n">
-        <v>8.380000000000001</v>
+        <v>17.72</v>
       </c>
       <c r="F13" t="n">
-        <v>1.89</v>
+        <v>4.52</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
+          <t>2-0</t>
+        </is>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>95.45</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>82.25</v>
+      </c>
+      <c r="J13" t="n">
+        <v>22.24</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>71.34</v>
+      </c>
+      <c r="L13" t="n">
+        <v>44.83</v>
+      </c>
+      <c r="M13" s="2" t="n">
+        <v>76.38</v>
+      </c>
+      <c r="N13" s="2" t="n">
+        <v>89.51000000000001</v>
+      </c>
+      <c r="O13" t="n">
+        <v>27.51</v>
+      </c>
+      <c r="P13" t="n">
+        <v>63.58</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>30.56</v>
+      </c>
+      <c r="R13" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>2-0</t>
+        </is>
+      </c>
+      <c r="T13" s="2" t="n">
+        <v>94.14</v>
+      </c>
+      <c r="U13" t="n">
+        <v>65.86</v>
+      </c>
+      <c r="V13" t="n">
+        <v>32.84</v>
+      </c>
+      <c r="W13" s="2" t="n">
+        <v>80.09999999999999</v>
+      </c>
+      <c r="X13" t="n">
+        <v>31.07</v>
+      </c>
+      <c r="Y13" s="2" t="n">
+        <v>87.8</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>30.51</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>62.17</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>5.22</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>64.79000000000001</v>
+      </c>
+      <c r="AD13" s="2" t="n">
+        <v>99.34999999999999</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>UNL</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Lithuania</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Finland</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>47.14</v>
+      </c>
+      <c r="E14" t="n">
+        <v>40.66</v>
+      </c>
+      <c r="F14" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>0-0</t>
+        </is>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>87.8</v>
+      </c>
+      <c r="I14" t="n">
+        <v>59.34</v>
+      </c>
+      <c r="J14" t="n">
+        <v>52.86</v>
+      </c>
+      <c r="K14" t="n">
+        <v>35.51</v>
+      </c>
+      <c r="L14" t="n">
+        <v>12.55</v>
+      </c>
+      <c r="M14" s="2" t="n">
+        <v>96.42</v>
+      </c>
+      <c r="N14" s="2" t="n">
+        <v>99.16</v>
+      </c>
+      <c r="O14" t="n">
+        <v>17.52</v>
+      </c>
+      <c r="P14" t="n">
+        <v>7.99</v>
+      </c>
+      <c r="Q14" s="2" t="n">
+        <v>71.51000000000001</v>
+      </c>
+      <c r="R14" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>0-0</t>
+        </is>
+      </c>
+      <c r="T14" s="2" t="n">
+        <v>79.5</v>
+      </c>
+      <c r="U14" t="n">
+        <v>28.49</v>
+      </c>
+      <c r="V14" s="2" t="n">
+        <v>92.01000000000001</v>
+      </c>
+      <c r="W14" t="n">
+        <v>32.61</v>
+      </c>
+      <c r="X14" s="2" t="n">
+        <v>91.75</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>59.08</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>28.05</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>22.52</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>4.36</v>
+      </c>
+      <c r="AC14" s="2" t="n">
+        <v>93.81999999999999</v>
+      </c>
+      <c r="AD14" s="2" t="n">
+        <v>99.53</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>UNL</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Poland</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Malta</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>57.77</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>8-0</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>57.84</v>
+      </c>
+      <c r="I15" t="n">
+        <v>57.77</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="K15" t="n">
+        <v>57.6</v>
+      </c>
+      <c r="L15" t="n">
+        <v>56.7</v>
+      </c>
+      <c r="M15" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="N15" t="n">
+        <v>8.66</v>
+      </c>
+      <c r="O15" t="n">
+        <v>7.57</v>
+      </c>
+      <c r="P15" t="n">
+        <v>13.06</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="R15" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>4-0</t>
+        </is>
+      </c>
+      <c r="T15" t="n">
+        <v>13.15</v>
+      </c>
+      <c r="U15" t="n">
+        <v>13.05</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="W15" t="n">
+        <v>13.08</v>
+      </c>
+      <c r="X15" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>57.81</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>7.57</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>57.57</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>57.82</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>UNL</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Bosnia</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Cyprus</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>88.52</v>
+      </c>
+      <c r="E16" t="n">
+        <v>8</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
           <t>3-0</t>
         </is>
       </c>
-      <c r="H13" s="2" t="n">
-        <v>97.53</v>
-      </c>
-      <c r="I13" s="2" t="n">
-        <v>91.04000000000001</v>
-      </c>
-      <c r="J13" t="n">
-        <v>10.27</v>
-      </c>
-      <c r="K13" s="2" t="n">
-        <v>87.40000000000001</v>
-      </c>
-      <c r="L13" t="n">
-        <v>69.34999999999999</v>
-      </c>
-      <c r="M13" t="n">
-        <v>51.28</v>
-      </c>
-      <c r="N13" s="2" t="n">
-        <v>70.42</v>
-      </c>
-      <c r="O13" t="n">
-        <v>32.06</v>
-      </c>
-      <c r="P13" t="n">
+      <c r="H16" s="2" t="n">
+        <v>96.52</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>91.03999999999999</v>
+      </c>
+      <c r="J16" t="n">
+        <v>10.52</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>90.56</v>
+      </c>
+      <c r="L16" s="2" t="n">
+        <v>75.84</v>
+      </c>
+      <c r="M16" t="n">
+        <v>42.54</v>
+      </c>
+      <c r="N16" t="n">
+        <v>62.07</v>
+      </c>
+      <c r="O16" t="n">
+        <v>41.46</v>
+      </c>
+      <c r="P16" s="2" t="n">
+        <v>74.09999999999999</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>22.58</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>1-0</t>
+        </is>
+      </c>
+      <c r="T16" s="2" t="n">
+        <v>96.67999999999999</v>
+      </c>
+      <c r="U16" s="2" t="n">
+        <v>74.19</v>
+      </c>
+      <c r="V16" t="n">
+        <v>22.67</v>
+      </c>
+      <c r="W16" s="2" t="n">
+        <v>79.16</v>
+      </c>
+      <c r="X16" t="n">
+        <v>42.93</v>
+      </c>
+      <c r="Y16" s="2" t="n">
+        <v>95.97</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>42.4</v>
+      </c>
+      <c r="AA16" s="2" t="n">
+        <v>85.27</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>10.75</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>32.4</v>
+      </c>
+      <c r="AD16" s="2" t="n">
+        <v>97.14</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>UNL</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>San Marino</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Romania</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="E17" t="n">
+        <v>7.14</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>91.47</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>0-3</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>8.08</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>92.41</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>98.61</v>
+      </c>
+      <c r="K17" s="2" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="L17" t="n">
+        <v>63.58</v>
+      </c>
+      <c r="M17" t="n">
+        <v>58.06</v>
+      </c>
+      <c r="N17" s="2" t="n">
+        <v>76.28</v>
+      </c>
+      <c r="O17" t="n">
+        <v>18.73</v>
+      </c>
+      <c r="P17" t="n">
+        <v>-0</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>17.08</v>
+      </c>
+      <c r="R17" s="2" t="n">
+        <v>79.51000000000001</v>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="T17" t="n">
+        <v>17.08</v>
+      </c>
+      <c r="U17" s="2" t="n">
+        <v>79.51000000000001</v>
+      </c>
+      <c r="V17" s="2" t="n">
+        <v>96.59</v>
+      </c>
+      <c r="W17" s="2" t="n">
+        <v>79.51000000000001</v>
+      </c>
+      <c r="X17" t="n">
+        <v>47.27</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>19.35</v>
+      </c>
+      <c r="Z17" s="2" t="n">
+        <v>94.95999999999999</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>2.02</v>
+      </c>
+      <c r="AB17" s="2" t="n">
+        <v>80.83</v>
+      </c>
+      <c r="AC17" s="2" t="n">
+        <v>99.41</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>UNL</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Albania</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Andorra</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>92.91</v>
+      </c>
+      <c r="E18" t="n">
+        <v>6.92</v>
+      </c>
+      <c r="F18" t="n">
         <v>0</v>
       </c>
-      <c r="Q13" t="n">
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>2-0</t>
+        </is>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>99.83</v>
+      </c>
+      <c r="I18" s="2" t="n">
+        <v>92.91</v>
+      </c>
+      <c r="J18" t="n">
+        <v>6.92</v>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>74.43000000000001</v>
+      </c>
+      <c r="L18" t="n">
+        <v>49.76</v>
+      </c>
+      <c r="M18" s="2" t="n">
+        <v>72.04000000000001</v>
+      </c>
+      <c r="N18" s="2" t="n">
+        <v>86.70999999999999</v>
+      </c>
+      <c r="O18" t="n">
         <v>0</v>
       </c>
-      <c r="R13" t="n">
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>0-0</t>
+        </is>
+      </c>
+      <c r="T18" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0</v>
+      </c>
+      <c r="V18" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="W18" t="n">
+        <v>0</v>
+      </c>
+      <c r="X18" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y18" s="2" t="n">
+        <v>92.91</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="2" t="n">
+        <v>74.43000000000001</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>50.06</v>
+      </c>
+      <c r="AD18" s="2" t="n">
+        <v>99.81999999999999</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>UNL</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Latvia</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>77.02</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>6-0</t>
+        </is>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>77.33999999999999</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>77.03999999999999</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>76.55</v>
+      </c>
+      <c r="L19" s="2" t="n">
+        <v>74.03</v>
+      </c>
+      <c r="M19" t="n">
+        <v>9.050000000000001</v>
+      </c>
+      <c r="N19" t="n">
+        <v>18.81</v>
+      </c>
+      <c r="O19" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="P19" s="2" t="n">
+        <v>74.3</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="R19" t="n">
         <v>-0</v>
       </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>4-0</t>
-        </is>
-      </c>
-      <c r="T13" t="n">
-        <v>0</v>
-      </c>
-      <c r="U13" t="n">
-        <v>0</v>
-      </c>
-      <c r="V13" t="n">
-        <v>0</v>
-      </c>
-      <c r="W13" t="n">
-        <v>0</v>
-      </c>
-      <c r="X13" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="2" t="n">
-        <v>95.38</v>
-      </c>
-      <c r="Z13" t="n">
-        <v>32.96</v>
-      </c>
-      <c r="AA13" s="2" t="n">
-        <v>82.41</v>
-      </c>
-      <c r="AB13" t="n">
-        <v>6.19</v>
-      </c>
-      <c r="AC13" t="n">
-        <v>37.81</v>
-      </c>
-      <c r="AD13" s="2" t="n">
-        <v>98.62</v>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>3-0</t>
+        </is>
+      </c>
+      <c r="T19" s="2" t="n">
+        <v>78.47</v>
+      </c>
+      <c r="U19" s="2" t="n">
+        <v>74.3</v>
+      </c>
+      <c r="V19" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="W19" s="2" t="n">
+        <v>74.3</v>
+      </c>
+      <c r="X19" t="n">
+        <v>17.43</v>
+      </c>
+      <c r="Y19" s="2" t="n">
+        <v>77.23999999999999</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>13.51</v>
+      </c>
+      <c r="AA19" s="2" t="n">
+        <v>76.38</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>3.86</v>
+      </c>
+      <c r="AD19" s="2" t="n">
+        <v>77.29000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>